<commit_message>
july 23 babine update
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9236AB5D-239B-4D49-9FC9-9561F11EF2D8}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C42306D-C888-425A-952A-C228710B4F7B}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1880" windowWidth="19200" windowHeight="11180" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="-22830" yWindow="6105" windowWidth="19200" windowHeight="11175" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -175,6 +175,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,10 +501,10 @@
   <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L22" sqref="L22"/>
+      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" ref="N2:N22" si="0">B2+M2</f>
+        <f t="shared" ref="N2:N23" si="0">B2+M2</f>
         <v>0</v>
       </c>
       <c r="O2" s="1">
@@ -652,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M22" si="2">I3+K3</f>
+        <f t="shared" ref="M3:M23" si="2">I3+K3</f>
         <v>0</v>
       </c>
       <c r="N3" s="2">
@@ -1023,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" ref="P10:P22" si="5">C10+J10</f>
+        <f t="shared" ref="P10:P23" si="5">C10+J10</f>
         <v>0</v>
       </c>
       <c r="Q10" s="1">
@@ -2081,6 +2085,60 @@
       <c r="A23" s="3">
         <v>45495</v>
       </c>
+      <c r="B23">
+        <v>11449</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" ref="L23" si="9">L22+B23</f>
+        <v>21800</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" ref="M23" si="10">I23+K23</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" ref="N23" si="11">B23+M23</f>
+        <v>11449</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" ref="O23" si="12">O22+N23</f>
+        <v>21800</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" ref="P23" si="13">C23+J23</f>
+        <v>200</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" ref="Q23" si="14">P23+Q22</f>
+        <v>366</v>
+      </c>
       <c r="R23" s="1">
         <v>19763</v>
       </c>
@@ -2491,11 +2549,11 @@
         <v>18790.8</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" ref="T36:U51" si="9">T35+R36</f>
+        <f t="shared" ref="T36:U51" si="15">T35+R36</f>
         <v>520442</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>179104.5853174603</v>
       </c>
       <c r="V36" s="1">
@@ -2522,11 +2580,11 @@
         <v>25713.3</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>550390</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>204817.88531746028</v>
       </c>
       <c r="V37" s="1">
@@ -2553,11 +2611,11 @@
         <v>18006.400000000001</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>581098</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>222824.28531746028</v>
       </c>
       <c r="V38" s="1">
@@ -2584,11 +2642,11 @@
         <v>24560.3</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>605588</v>
       </c>
       <c r="U39" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>247384.58531746027</v>
       </c>
       <c r="V39" s="1">
@@ -2615,11 +2673,11 @@
         <v>22302.5</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>627171</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>269687.08531746024</v>
       </c>
       <c r="V40" s="1">
@@ -2646,11 +2704,11 @@
         <v>36342.400000000001</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>652373</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>306029.48531746026</v>
       </c>
       <c r="V41" s="1">
@@ -2677,11 +2735,11 @@
         <v>26445.363636363636</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>675506</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>332474.84895382391</v>
       </c>
       <c r="V42" s="1">
@@ -2708,11 +2766,11 @@
         <v>28798.363636363636</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>717110</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>361273.21259018756</v>
       </c>
       <c r="V43" s="1">
@@ -2739,11 +2797,11 @@
         <v>22717.545454545456</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>740207</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>383990.75804473303</v>
       </c>
       <c r="V44" s="1">
@@ -2770,11 +2828,11 @@
         <v>24761.090909090908</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>770155</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>408751.84895382391</v>
       </c>
       <c r="V45" s="1">
@@ -2801,11 +2859,11 @@
         <v>27668.909090909092</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>813557</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>436420.75804473303</v>
       </c>
       <c r="V46" s="1">
@@ -2832,11 +2890,11 @@
         <v>28715</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>849071</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>465135.75804473303</v>
       </c>
       <c r="V47" s="1">
@@ -2863,11 +2921,11 @@
         <v>19741.18181818182</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>891191</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>484876.93986291485</v>
       </c>
       <c r="V48" s="1">
@@ -2894,11 +2952,11 @@
         <v>24994.81818181818</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>963510</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>509871.75804473303</v>
       </c>
       <c r="V49" s="1">
@@ -2925,11 +2983,11 @@
         <v>30512.18181818182</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1014593</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>540383.93986291485</v>
       </c>
       <c r="V50" s="1">
@@ -2956,11 +3014,11 @@
         <v>29755.272727272728</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1077884</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>570139.21259018756</v>
       </c>
       <c r="V51" s="1">
@@ -2987,11 +3045,11 @@
         <v>29568.909090909092</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" ref="T52:U67" si="10">T51+R52</f>
+        <f t="shared" ref="T52:U67" si="16">T51+R52</f>
         <v>1114483</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>599708.12168109661</v>
       </c>
       <c r="V52" s="1">
@@ -3018,11 +3076,11 @@
         <v>27004.636363636364</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1174452</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>626712.75804473297</v>
       </c>
       <c r="V53" s="1">
@@ -3049,11 +3107,11 @@
         <v>26730.909090909092</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1202504</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>653443.66713564203</v>
       </c>
       <c r="V54" s="1">
@@ -3080,11 +3138,11 @@
         <v>22068.454545454544</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1277668</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>675512.12168109661</v>
       </c>
       <c r="V55" s="1">
@@ -3111,11 +3169,11 @@
         <v>24809.363636363636</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1370228</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>700321.48531746026</v>
       </c>
       <c r="V56" s="1">
@@ -3142,11 +3200,11 @@
         <v>28342.545454545456</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1440848</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>728664.03077200567</v>
       </c>
       <c r="V57" s="1">
@@ -3173,11 +3231,11 @@
         <v>26309.272727272728</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1497008</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>754973.30349927838</v>
       </c>
       <c r="V58" s="1">
@@ -3204,11 +3262,11 @@
         <v>23571.727272727272</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1540279</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>778545.03077200567</v>
       </c>
       <c r="V59" s="1">
@@ -3235,11 +3293,11 @@
         <v>21629.454545454544</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1594464</v>
       </c>
       <c r="U60" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>800174.48531746026</v>
       </c>
       <c r="V60" s="1">
@@ -3266,11 +3324,11 @@
         <v>21511.909090909092</v>
       </c>
       <c r="T61" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1642593</v>
       </c>
       <c r="U61" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>821686.39440836932</v>
       </c>
       <c r="V61" s="1">
@@ -3297,11 +3355,11 @@
         <v>19461.272727272728</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1678981</v>
       </c>
       <c r="U62" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>841147.66713564203</v>
       </c>
       <c r="V62" s="1">
@@ -3328,11 +3386,11 @@
         <v>17916.636363636364</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1711287</v>
       </c>
       <c r="U63" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>859064.30349927838</v>
       </c>
       <c r="V63" s="1">
@@ -3359,11 +3417,11 @@
         <v>17763.909090909092</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1744119</v>
       </c>
       <c r="U64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>876828.21259018744</v>
       </c>
       <c r="V64" s="1">
@@ -3390,11 +3448,11 @@
         <v>17535.090909090908</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1768866</v>
       </c>
       <c r="U65" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>894363.30349927838</v>
       </c>
       <c r="V65" s="1">
@@ -3421,11 +3479,11 @@
         <v>17130.18181818182</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1794920</v>
       </c>
       <c r="U66" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>911493.48531746014</v>
       </c>
       <c r="V66" s="1">
@@ -3452,11 +3510,11 @@
         <v>17186.363636363636</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1816116</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>928679.84895382379</v>
       </c>
       <c r="V67" s="1">
@@ -3483,11 +3541,11 @@
         <v>14679.636363636364</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" ref="T68:U83" si="11">T67+R68</f>
+        <f t="shared" ref="T68:U83" si="17">T67+R68</f>
         <v>1846521</v>
       </c>
       <c r="U68" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>943359.48531746014</v>
       </c>
       <c r="V68" s="1">
@@ -3514,11 +3572,11 @@
         <v>15690.818181818182</v>
       </c>
       <c r="T69" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1878833</v>
       </c>
       <c r="U69" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>959050.30349927838</v>
       </c>
       <c r="V69" s="1">
@@ -3545,11 +3603,11 @@
         <v>14967.545454545454</v>
       </c>
       <c r="T70" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1901010</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>974017.84895382379</v>
       </c>
       <c r="V70" s="1">
@@ -3576,11 +3634,11 @@
         <v>14546.818181818182</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1914981</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>988564.66713564203</v>
       </c>
       <c r="V71" s="1">
@@ -3607,11 +3665,11 @@
         <v>13876.272727272728</v>
       </c>
       <c r="T72" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1928616</v>
       </c>
       <c r="U72" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1002440.9398629147</v>
       </c>
       <c r="V72" s="1">
@@ -3638,11 +3696,11 @@
         <v>12522.363636363636</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1938412</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1014963.3034992784</v>
       </c>
       <c r="V73" s="1">
@@ -3669,11 +3727,11 @@
         <v>12105.636363636364</v>
       </c>
       <c r="T74" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1946010</v>
       </c>
       <c r="U74" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1027068.9398629147</v>
       </c>
       <c r="V74" s="1">
@@ -3700,11 +3758,11 @@
         <v>11272.545454545454</v>
       </c>
       <c r="T75" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1953188</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1038341.4853174601</v>
       </c>
       <c r="V75" s="1">
@@ -3731,11 +3789,11 @@
         <v>9771.0909090909099</v>
       </c>
       <c r="T76" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1962346</v>
       </c>
       <c r="U76" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1048112.5762265511</v>
       </c>
       <c r="V76" s="1">
@@ -3762,11 +3820,11 @@
         <v>7589.909090909091</v>
       </c>
       <c r="T77" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1973666</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1055702.4853174603</v>
       </c>
       <c r="V77" s="1">
@@ -3793,11 +3851,11 @@
         <v>8318.545454545454</v>
       </c>
       <c r="T78" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1981697</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1064021.0307720057</v>
       </c>
       <c r="V78" s="1">
@@ -3824,11 +3882,11 @@
         <v>7405.727272727273</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1991144</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1071426.758044733</v>
       </c>
       <c r="V79" s="1">
@@ -3855,11 +3913,11 @@
         <v>7004.181818181818</v>
       </c>
       <c r="T80" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2001289</v>
       </c>
       <c r="U80" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1078430.9398629148</v>
       </c>
       <c r="V80" s="1">
@@ -3886,11 +3944,11 @@
         <v>6677.818181818182</v>
       </c>
       <c r="T81" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2013289</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1085108.758044733</v>
       </c>
       <c r="V81" s="1">
@@ -3917,11 +3975,11 @@
         <v>6140.454545454545</v>
       </c>
       <c r="T82" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2026172</v>
       </c>
       <c r="U82" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1091249.2125901876</v>
       </c>
       <c r="V82" s="1">
@@ -3948,11 +4006,11 @@
         <v>6411.4</v>
       </c>
       <c r="T83" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2032538</v>
       </c>
       <c r="U83" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1097660.6125901875</v>
       </c>
       <c r="V83" s="1">
@@ -3979,11 +4037,11 @@
         <v>6189.6</v>
       </c>
       <c r="T84" s="1">
-        <f t="shared" ref="T84:U99" si="12">T83+R84</f>
+        <f t="shared" ref="T84:U99" si="18">T83+R84</f>
         <v>2036693</v>
       </c>
       <c r="U84" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1103850.2125901876</v>
       </c>
       <c r="V84" s="1">
@@ -4010,11 +4068,11 @@
         <v>4314.3999999999996</v>
       </c>
       <c r="T85" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2039343</v>
       </c>
       <c r="U85" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1108164.6125901875</v>
       </c>
       <c r="V85" s="1">
@@ -4041,11 +4099,11 @@
         <v>3802.6</v>
       </c>
       <c r="T86" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2043072</v>
       </c>
       <c r="U86" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1111967.2125901876</v>
       </c>
       <c r="V86" s="1">
@@ -4072,11 +4130,11 @@
         <v>3261.3333333333335</v>
       </c>
       <c r="T87" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2045727</v>
       </c>
       <c r="U87" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1115228.5459235208</v>
       </c>
       <c r="V87" s="1">
@@ -4103,11 +4161,11 @@
         <v>2728.4444444444443</v>
       </c>
       <c r="T88" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2047725</v>
       </c>
       <c r="U88" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1117956.9903679653</v>
       </c>
       <c r="V88" s="1">
@@ -4134,11 +4192,11 @@
         <v>2059.7777777777778</v>
       </c>
       <c r="T89" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2049017</v>
       </c>
       <c r="U89" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1120016.7681457431</v>
       </c>
       <c r="V89" s="1">
@@ -4165,11 +4223,11 @@
         <v>1764.2222222222222</v>
       </c>
       <c r="T90" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2049846</v>
       </c>
       <c r="U90" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1121780.9903679653</v>
       </c>
       <c r="V90" s="1">
@@ -4196,11 +4254,11 @@
         <v>1664.125</v>
       </c>
       <c r="T91" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2051014</v>
       </c>
       <c r="U91" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1123445.1153679653</v>
       </c>
       <c r="V91" s="1">
@@ -4227,11 +4285,11 @@
         <v>1687.375</v>
       </c>
       <c r="T92" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2051949</v>
       </c>
       <c r="U92" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1125132.4903679653</v>
       </c>
       <c r="V92" s="1">
@@ -4258,11 +4316,11 @@
         <v>868.83333333333337</v>
       </c>
       <c r="T93" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U93" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1126001.3237012986</v>
       </c>
       <c r="V93" s="1">
@@ -4286,11 +4344,11 @@
         <v>707.66666666666663</v>
       </c>
       <c r="T94" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U94" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1126708.9903679653</v>
       </c>
       <c r="V94" s="1">
@@ -4314,11 +4372,11 @@
         <v>440</v>
       </c>
       <c r="T95" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U95" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1127148.9903679653</v>
       </c>
       <c r="V95" s="1">
@@ -4342,11 +4400,11 @@
         <v>720.66666666666663</v>
       </c>
       <c r="T96" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U96" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1127869.6570346321</v>
       </c>
       <c r="V96" s="1">
@@ -4370,11 +4428,11 @@
         <v>238</v>
       </c>
       <c r="T97" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U97" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1128107.6570346321</v>
       </c>
       <c r="V97" s="1">
@@ -4398,11 +4456,11 @@
         <v>323</v>
       </c>
       <c r="T98" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U98" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1128430.6570346321</v>
       </c>
       <c r="V98" s="1">
@@ -4426,11 +4484,11 @@
         <v>250</v>
       </c>
       <c r="T99" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>2052845</v>
       </c>
       <c r="U99" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V99" s="1">
@@ -4451,11 +4509,11 @@
         <v>45572</v>
       </c>
       <c r="T100" s="1">
-        <f t="shared" ref="T100:U108" si="13">T99+R100</f>
+        <f t="shared" ref="T100:U108" si="19">T99+R100</f>
         <v>2052845</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V100" s="1">
@@ -4476,11 +4534,11 @@
         <v>45573</v>
       </c>
       <c r="T101" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V101" s="1">
@@ -4495,11 +4553,11 @@
         <v>45574</v>
       </c>
       <c r="T102" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V102" s="1">
@@ -4514,11 +4572,11 @@
         <v>45575</v>
       </c>
       <c r="T103" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V103" s="1">
@@ -4533,11 +4591,11 @@
         <v>45576</v>
       </c>
       <c r="T104" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V104" s="1">
@@ -4552,11 +4610,11 @@
         <v>45577</v>
       </c>
       <c r="T105" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V105" s="1">
@@ -4571,11 +4629,11 @@
         <v>45578</v>
       </c>
       <c r="T106" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V106" s="1">
@@ -4590,11 +4648,11 @@
         <v>45579</v>
       </c>
       <c r="T107" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V107" s="1">
@@ -4609,11 +4667,11 @@
         <v>45580</v>
       </c>
       <c r="T108" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2052845</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V108" s="1">

</xml_diff>

<commit_message>
july 25 update 2
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C42306D-C888-425A-952A-C228710B4F7B}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65DE0EA0-ED75-4C24-B04E-0A65E04E1C3A}"/>
   <bookViews>
-    <workbookView xWindow="-22830" yWindow="6105" windowWidth="19200" windowHeight="11175" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="3760" yWindow="2060" windowWidth="19200" windowHeight="11180" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -175,10 +175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,10 +497,10 @@
   <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" ref="N2:N23" si="0">B2+M2</f>
+        <f t="shared" ref="N2:N22" si="0">B2+M2</f>
         <v>0</v>
       </c>
       <c r="O2" s="1">
@@ -656,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M23" si="2">I3+K3</f>
+        <f t="shared" ref="M3:M22" si="2">I3+K3</f>
         <v>0</v>
       </c>
       <c r="N3" s="2">
@@ -1027,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" ref="P10:P23" si="5">C10+J10</f>
+        <f t="shared" ref="P10:P22" si="5">C10+J10</f>
         <v>0</v>
       </c>
       <c r="Q10" s="1">
@@ -2120,11 +2116,11 @@
         <v>21800</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" ref="M23" si="10">I23+K23</f>
+        <f t="shared" ref="M23:M25" si="10">I23+K23</f>
         <v>0</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" ref="N23" si="11">B23+M23</f>
+        <f t="shared" ref="N23:N25" si="11">B23+M23</f>
         <v>11449</v>
       </c>
       <c r="O23" s="1">
@@ -2132,7 +2128,7 @@
         <v>21800</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" ref="P23" si="13">C23+J23</f>
+        <f t="shared" ref="P23:P25" si="13">C23+J23</f>
         <v>200</v>
       </c>
       <c r="Q23" s="1">
@@ -2170,6 +2166,60 @@
       <c r="A24" s="3">
         <v>45496</v>
       </c>
+      <c r="B24">
+        <v>25407</v>
+      </c>
+      <c r="C24">
+        <v>1060</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" ref="L24:L25" si="15">L23+B24</f>
+        <v>47207</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" ref="M24:M25" si="16">I24+K24</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" ref="N24:N25" si="17">B24+M24</f>
+        <v>25407</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" ref="O24:O25" si="18">O23+N24</f>
+        <v>47207</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" ref="P24:P25" si="19">C24+J24</f>
+        <v>1060</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" ref="Q24:Q25" si="20">P24+Q23</f>
+        <v>1426</v>
+      </c>
       <c r="R24" s="1">
         <v>12174</v>
       </c>
@@ -2201,6 +2251,60 @@
       <c r="A25" s="3">
         <v>45497</v>
       </c>
+      <c r="B25">
+        <v>13068</v>
+      </c>
+      <c r="C25">
+        <v>538</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>20</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="15"/>
+        <v>60275</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="17"/>
+        <v>13068</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="18"/>
+        <v>60275</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" si="19"/>
+        <v>538</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="20"/>
+        <v>1964</v>
+      </c>
       <c r="R25" s="1">
         <v>16576</v>
       </c>
@@ -2549,11 +2653,11 @@
         <v>18790.8</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" ref="T36:U51" si="15">T35+R36</f>
+        <f t="shared" ref="T36:U51" si="21">T35+R36</f>
         <v>520442</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>179104.5853174603</v>
       </c>
       <c r="V36" s="1">
@@ -2580,11 +2684,11 @@
         <v>25713.3</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>550390</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>204817.88531746028</v>
       </c>
       <c r="V37" s="1">
@@ -2611,11 +2715,11 @@
         <v>18006.400000000001</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>581098</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>222824.28531746028</v>
       </c>
       <c r="V38" s="1">
@@ -2642,11 +2746,11 @@
         <v>24560.3</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>605588</v>
       </c>
       <c r="U39" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>247384.58531746027</v>
       </c>
       <c r="V39" s="1">
@@ -2673,11 +2777,11 @@
         <v>22302.5</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>627171</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>269687.08531746024</v>
       </c>
       <c r="V40" s="1">
@@ -2704,11 +2808,11 @@
         <v>36342.400000000001</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>652373</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>306029.48531746026</v>
       </c>
       <c r="V41" s="1">
@@ -2735,11 +2839,11 @@
         <v>26445.363636363636</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>675506</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>332474.84895382391</v>
       </c>
       <c r="V42" s="1">
@@ -2766,11 +2870,11 @@
         <v>28798.363636363636</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>717110</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>361273.21259018756</v>
       </c>
       <c r="V43" s="1">
@@ -2797,11 +2901,11 @@
         <v>22717.545454545456</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>740207</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>383990.75804473303</v>
       </c>
       <c r="V44" s="1">
@@ -2828,11 +2932,11 @@
         <v>24761.090909090908</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>770155</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>408751.84895382391</v>
       </c>
       <c r="V45" s="1">
@@ -2859,11 +2963,11 @@
         <v>27668.909090909092</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>813557</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>436420.75804473303</v>
       </c>
       <c r="V46" s="1">
@@ -2890,11 +2994,11 @@
         <v>28715</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>849071</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>465135.75804473303</v>
       </c>
       <c r="V47" s="1">
@@ -2921,11 +3025,11 @@
         <v>19741.18181818182</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>891191</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>484876.93986291485</v>
       </c>
       <c r="V48" s="1">
@@ -2952,11 +3056,11 @@
         <v>24994.81818181818</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>963510</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>509871.75804473303</v>
       </c>
       <c r="V49" s="1">
@@ -2983,11 +3087,11 @@
         <v>30512.18181818182</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1014593</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>540383.93986291485</v>
       </c>
       <c r="V50" s="1">
@@ -3014,11 +3118,11 @@
         <v>29755.272727272728</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1077884</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>570139.21259018756</v>
       </c>
       <c r="V51" s="1">
@@ -3045,11 +3149,11 @@
         <v>29568.909090909092</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" ref="T52:U67" si="16">T51+R52</f>
+        <f t="shared" ref="T52:U67" si="22">T51+R52</f>
         <v>1114483</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>599708.12168109661</v>
       </c>
       <c r="V52" s="1">
@@ -3076,11 +3180,11 @@
         <v>27004.636363636364</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1174452</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>626712.75804473297</v>
       </c>
       <c r="V53" s="1">
@@ -3107,11 +3211,11 @@
         <v>26730.909090909092</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1202504</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>653443.66713564203</v>
       </c>
       <c r="V54" s="1">
@@ -3138,11 +3242,11 @@
         <v>22068.454545454544</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1277668</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>675512.12168109661</v>
       </c>
       <c r="V55" s="1">
@@ -3169,11 +3273,11 @@
         <v>24809.363636363636</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1370228</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>700321.48531746026</v>
       </c>
       <c r="V56" s="1">
@@ -3200,11 +3304,11 @@
         <v>28342.545454545456</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1440848</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>728664.03077200567</v>
       </c>
       <c r="V57" s="1">
@@ -3231,11 +3335,11 @@
         <v>26309.272727272728</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1497008</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>754973.30349927838</v>
       </c>
       <c r="V58" s="1">
@@ -3262,11 +3366,11 @@
         <v>23571.727272727272</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1540279</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>778545.03077200567</v>
       </c>
       <c r="V59" s="1">
@@ -3293,11 +3397,11 @@
         <v>21629.454545454544</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1594464</v>
       </c>
       <c r="U60" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>800174.48531746026</v>
       </c>
       <c r="V60" s="1">
@@ -3324,11 +3428,11 @@
         <v>21511.909090909092</v>
       </c>
       <c r="T61" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1642593</v>
       </c>
       <c r="U61" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>821686.39440836932</v>
       </c>
       <c r="V61" s="1">
@@ -3355,11 +3459,11 @@
         <v>19461.272727272728</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1678981</v>
       </c>
       <c r="U62" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>841147.66713564203</v>
       </c>
       <c r="V62" s="1">
@@ -3386,11 +3490,11 @@
         <v>17916.636363636364</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1711287</v>
       </c>
       <c r="U63" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>859064.30349927838</v>
       </c>
       <c r="V63" s="1">
@@ -3417,11 +3521,11 @@
         <v>17763.909090909092</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1744119</v>
       </c>
       <c r="U64" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>876828.21259018744</v>
       </c>
       <c r="V64" s="1">
@@ -3448,11 +3552,11 @@
         <v>17535.090909090908</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1768866</v>
       </c>
       <c r="U65" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>894363.30349927838</v>
       </c>
       <c r="V65" s="1">
@@ -3479,11 +3583,11 @@
         <v>17130.18181818182</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1794920</v>
       </c>
       <c r="U66" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>911493.48531746014</v>
       </c>
       <c r="V66" s="1">
@@ -3510,11 +3614,11 @@
         <v>17186.363636363636</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1816116</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>928679.84895382379</v>
       </c>
       <c r="V67" s="1">
@@ -3541,11 +3645,11 @@
         <v>14679.636363636364</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" ref="T68:U83" si="17">T67+R68</f>
+        <f t="shared" ref="T68:U83" si="23">T67+R68</f>
         <v>1846521</v>
       </c>
       <c r="U68" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>943359.48531746014</v>
       </c>
       <c r="V68" s="1">
@@ -3572,11 +3676,11 @@
         <v>15690.818181818182</v>
       </c>
       <c r="T69" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1878833</v>
       </c>
       <c r="U69" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>959050.30349927838</v>
       </c>
       <c r="V69" s="1">
@@ -3603,11 +3707,11 @@
         <v>14967.545454545454</v>
       </c>
       <c r="T70" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1901010</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>974017.84895382379</v>
       </c>
       <c r="V70" s="1">
@@ -3634,11 +3738,11 @@
         <v>14546.818181818182</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1914981</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>988564.66713564203</v>
       </c>
       <c r="V71" s="1">
@@ -3665,11 +3769,11 @@
         <v>13876.272727272728</v>
       </c>
       <c r="T72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1928616</v>
       </c>
       <c r="U72" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1002440.9398629147</v>
       </c>
       <c r="V72" s="1">
@@ -3696,11 +3800,11 @@
         <v>12522.363636363636</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1938412</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1014963.3034992784</v>
       </c>
       <c r="V73" s="1">
@@ -3727,11 +3831,11 @@
         <v>12105.636363636364</v>
       </c>
       <c r="T74" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1946010</v>
       </c>
       <c r="U74" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1027068.9398629147</v>
       </c>
       <c r="V74" s="1">
@@ -3758,11 +3862,11 @@
         <v>11272.545454545454</v>
       </c>
       <c r="T75" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1953188</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1038341.4853174601</v>
       </c>
       <c r="V75" s="1">
@@ -3789,11 +3893,11 @@
         <v>9771.0909090909099</v>
       </c>
       <c r="T76" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1962346</v>
       </c>
       <c r="U76" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1048112.5762265511</v>
       </c>
       <c r="V76" s="1">
@@ -3820,11 +3924,11 @@
         <v>7589.909090909091</v>
       </c>
       <c r="T77" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1973666</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1055702.4853174603</v>
       </c>
       <c r="V77" s="1">
@@ -3851,11 +3955,11 @@
         <v>8318.545454545454</v>
       </c>
       <c r="T78" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1981697</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1064021.0307720057</v>
       </c>
       <c r="V78" s="1">
@@ -3882,11 +3986,11 @@
         <v>7405.727272727273</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1991144</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1071426.758044733</v>
       </c>
       <c r="V79" s="1">
@@ -3913,11 +4017,11 @@
         <v>7004.181818181818</v>
       </c>
       <c r="T80" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>2001289</v>
       </c>
       <c r="U80" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1078430.9398629148</v>
       </c>
       <c r="V80" s="1">
@@ -3944,11 +4048,11 @@
         <v>6677.818181818182</v>
       </c>
       <c r="T81" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>2013289</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1085108.758044733</v>
       </c>
       <c r="V81" s="1">
@@ -3975,11 +4079,11 @@
         <v>6140.454545454545</v>
       </c>
       <c r="T82" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>2026172</v>
       </c>
       <c r="U82" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1091249.2125901876</v>
       </c>
       <c r="V82" s="1">
@@ -4006,11 +4110,11 @@
         <v>6411.4</v>
       </c>
       <c r="T83" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>2032538</v>
       </c>
       <c r="U83" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>1097660.6125901875</v>
       </c>
       <c r="V83" s="1">
@@ -4037,11 +4141,11 @@
         <v>6189.6</v>
       </c>
       <c r="T84" s="1">
-        <f t="shared" ref="T84:U99" si="18">T83+R84</f>
+        <f t="shared" ref="T84:U99" si="24">T83+R84</f>
         <v>2036693</v>
       </c>
       <c r="U84" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1103850.2125901876</v>
       </c>
       <c r="V84" s="1">
@@ -4068,11 +4172,11 @@
         <v>4314.3999999999996</v>
       </c>
       <c r="T85" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2039343</v>
       </c>
       <c r="U85" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1108164.6125901875</v>
       </c>
       <c r="V85" s="1">
@@ -4099,11 +4203,11 @@
         <v>3802.6</v>
       </c>
       <c r="T86" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2043072</v>
       </c>
       <c r="U86" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1111967.2125901876</v>
       </c>
       <c r="V86" s="1">
@@ -4130,11 +4234,11 @@
         <v>3261.3333333333335</v>
       </c>
       <c r="T87" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2045727</v>
       </c>
       <c r="U87" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1115228.5459235208</v>
       </c>
       <c r="V87" s="1">
@@ -4161,11 +4265,11 @@
         <v>2728.4444444444443</v>
       </c>
       <c r="T88" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2047725</v>
       </c>
       <c r="U88" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1117956.9903679653</v>
       </c>
       <c r="V88" s="1">
@@ -4192,11 +4296,11 @@
         <v>2059.7777777777778</v>
       </c>
       <c r="T89" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2049017</v>
       </c>
       <c r="U89" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1120016.7681457431</v>
       </c>
       <c r="V89" s="1">
@@ -4223,11 +4327,11 @@
         <v>1764.2222222222222</v>
       </c>
       <c r="T90" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2049846</v>
       </c>
       <c r="U90" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1121780.9903679653</v>
       </c>
       <c r="V90" s="1">
@@ -4254,11 +4358,11 @@
         <v>1664.125</v>
       </c>
       <c r="T91" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2051014</v>
       </c>
       <c r="U91" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1123445.1153679653</v>
       </c>
       <c r="V91" s="1">
@@ -4285,11 +4389,11 @@
         <v>1687.375</v>
       </c>
       <c r="T92" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2051949</v>
       </c>
       <c r="U92" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1125132.4903679653</v>
       </c>
       <c r="V92" s="1">
@@ -4316,11 +4420,11 @@
         <v>868.83333333333337</v>
       </c>
       <c r="T93" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U93" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1126001.3237012986</v>
       </c>
       <c r="V93" s="1">
@@ -4344,11 +4448,11 @@
         <v>707.66666666666663</v>
       </c>
       <c r="T94" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U94" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1126708.9903679653</v>
       </c>
       <c r="V94" s="1">
@@ -4372,11 +4476,11 @@
         <v>440</v>
       </c>
       <c r="T95" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U95" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1127148.9903679653</v>
       </c>
       <c r="V95" s="1">
@@ -4400,11 +4504,11 @@
         <v>720.66666666666663</v>
       </c>
       <c r="T96" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U96" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1127869.6570346321</v>
       </c>
       <c r="V96" s="1">
@@ -4428,11 +4532,11 @@
         <v>238</v>
       </c>
       <c r="T97" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U97" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1128107.6570346321</v>
       </c>
       <c r="V97" s="1">
@@ -4456,11 +4560,11 @@
         <v>323</v>
       </c>
       <c r="T98" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U98" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1128430.6570346321</v>
       </c>
       <c r="V98" s="1">
@@ -4484,11 +4588,11 @@
         <v>250</v>
       </c>
       <c r="T99" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>2052845</v>
       </c>
       <c r="U99" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V99" s="1">
@@ -4509,11 +4613,11 @@
         <v>45572</v>
       </c>
       <c r="T100" s="1">
-        <f t="shared" ref="T100:U108" si="19">T99+R100</f>
+        <f t="shared" ref="T100:U108" si="25">T99+R100</f>
         <v>2052845</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V100" s="1">
@@ -4534,11 +4638,11 @@
         <v>45573</v>
       </c>
       <c r="T101" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V101" s="1">
@@ -4553,11 +4657,11 @@
         <v>45574</v>
       </c>
       <c r="T102" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V102" s="1">
@@ -4572,11 +4676,11 @@
         <v>45575</v>
       </c>
       <c r="T103" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V103" s="1">
@@ -4591,11 +4695,11 @@
         <v>45576</v>
       </c>
       <c r="T104" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V104" s="1">
@@ -4610,11 +4714,11 @@
         <v>45577</v>
       </c>
       <c r="T105" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V105" s="1">
@@ -4629,11 +4733,11 @@
         <v>45578</v>
       </c>
       <c r="T106" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V106" s="1">
@@ -4648,11 +4752,11 @@
         <v>45579</v>
       </c>
       <c r="T107" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V107" s="1">
@@ -4667,11 +4771,11 @@
         <v>45580</v>
       </c>
       <c r="T108" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>2052845</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V108" s="1">

</xml_diff>

<commit_message>
july 27 update update
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65DE0EA0-ED75-4C24-B04E-0A65E04E1C3A}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A0A3637-8828-4E43-BD53-AF3D892F2817}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2060" windowWidth="19200" windowHeight="11180" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="2530" yWindow="1660" windowWidth="19200" windowHeight="11180" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -175,6 +175,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,10 +501,10 @@
   <dimension ref="A1:Y108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O25" sqref="O25"/>
+      <selection pane="bottomRight" activeCell="L25" sqref="L25:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2116,11 +2120,11 @@
         <v>21800</v>
       </c>
       <c r="M23" s="1">
-        <f t="shared" ref="M23:M25" si="10">I23+K23</f>
+        <f t="shared" ref="M23" si="10">I23+K23</f>
         <v>0</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" ref="N23:N25" si="11">B23+M23</f>
+        <f t="shared" ref="N23" si="11">B23+M23</f>
         <v>11449</v>
       </c>
       <c r="O23" s="1">
@@ -2128,7 +2132,7 @@
         <v>21800</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" ref="P23:P25" si="13">C23+J23</f>
+        <f t="shared" ref="P23" si="13">C23+J23</f>
         <v>200</v>
       </c>
       <c r="Q23" s="1">
@@ -2201,11 +2205,11 @@
         <v>47207</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" ref="M24:M25" si="16">I24+K24</f>
+        <f t="shared" ref="M24:M26" si="16">I24+K24</f>
         <v>0</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" ref="N24:N25" si="17">B24+M24</f>
+        <f t="shared" ref="N24:N26" si="17">B24+M24</f>
         <v>25407</v>
       </c>
       <c r="O24" s="1">
@@ -2213,7 +2217,7 @@
         <v>47207</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" ref="P24:P25" si="19">C24+J24</f>
+        <f t="shared" ref="P24:P26" si="19">C24+J24</f>
         <v>1060</v>
       </c>
       <c r="Q24" s="1">
@@ -2336,6 +2340,60 @@
       <c r="A26" s="3">
         <v>45498</v>
       </c>
+      <c r="B26">
+        <v>15166</v>
+      </c>
+      <c r="C26">
+        <v>801</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" ref="L26" si="21">L25+B26</f>
+        <v>75441</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" ref="M26" si="22">I26+K26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" ref="N26" si="23">B26+M26</f>
+        <v>15166</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" ref="O26" si="24">O25+N26</f>
+        <v>75441</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" ref="P26" si="25">C26+J26</f>
+        <v>801</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" ref="Q26" si="26">P26+Q25</f>
+        <v>2765</v>
+      </c>
       <c r="R26" s="1">
         <v>18566</v>
       </c>
@@ -2653,11 +2711,11 @@
         <v>18790.8</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" ref="T36:U51" si="21">T35+R36</f>
+        <f t="shared" ref="T36:U51" si="27">T35+R36</f>
         <v>520442</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>179104.5853174603</v>
       </c>
       <c r="V36" s="1">
@@ -2684,11 +2742,11 @@
         <v>25713.3</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>550390</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>204817.88531746028</v>
       </c>
       <c r="V37" s="1">
@@ -2715,11 +2773,11 @@
         <v>18006.400000000001</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>581098</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>222824.28531746028</v>
       </c>
       <c r="V38" s="1">
@@ -2746,11 +2804,11 @@
         <v>24560.3</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>605588</v>
       </c>
       <c r="U39" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>247384.58531746027</v>
       </c>
       <c r="V39" s="1">
@@ -2777,11 +2835,11 @@
         <v>22302.5</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>627171</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>269687.08531746024</v>
       </c>
       <c r="V40" s="1">
@@ -2808,11 +2866,11 @@
         <v>36342.400000000001</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>652373</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>306029.48531746026</v>
       </c>
       <c r="V41" s="1">
@@ -2839,11 +2897,11 @@
         <v>26445.363636363636</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>675506</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>332474.84895382391</v>
       </c>
       <c r="V42" s="1">
@@ -2870,11 +2928,11 @@
         <v>28798.363636363636</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>717110</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>361273.21259018756</v>
       </c>
       <c r="V43" s="1">
@@ -2901,11 +2959,11 @@
         <v>22717.545454545456</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>740207</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>383990.75804473303</v>
       </c>
       <c r="V44" s="1">
@@ -2932,11 +2990,11 @@
         <v>24761.090909090908</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>770155</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>408751.84895382391</v>
       </c>
       <c r="V45" s="1">
@@ -2963,11 +3021,11 @@
         <v>27668.909090909092</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>813557</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>436420.75804473303</v>
       </c>
       <c r="V46" s="1">
@@ -2994,11 +3052,11 @@
         <v>28715</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>849071</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>465135.75804473303</v>
       </c>
       <c r="V47" s="1">
@@ -3025,11 +3083,11 @@
         <v>19741.18181818182</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>891191</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>484876.93986291485</v>
       </c>
       <c r="V48" s="1">
@@ -3056,11 +3114,11 @@
         <v>24994.81818181818</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>963510</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>509871.75804473303</v>
       </c>
       <c r="V49" s="1">
@@ -3087,11 +3145,11 @@
         <v>30512.18181818182</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>1014593</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>540383.93986291485</v>
       </c>
       <c r="V50" s="1">
@@ -3118,11 +3176,11 @@
         <v>29755.272727272728</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>1077884</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>570139.21259018756</v>
       </c>
       <c r="V51" s="1">
@@ -3149,11 +3207,11 @@
         <v>29568.909090909092</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" ref="T52:U67" si="22">T51+R52</f>
+        <f t="shared" ref="T52:U67" si="28">T51+R52</f>
         <v>1114483</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>599708.12168109661</v>
       </c>
       <c r="V52" s="1">
@@ -3180,11 +3238,11 @@
         <v>27004.636363636364</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1174452</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>626712.75804473297</v>
       </c>
       <c r="V53" s="1">
@@ -3211,11 +3269,11 @@
         <v>26730.909090909092</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1202504</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>653443.66713564203</v>
       </c>
       <c r="V54" s="1">
@@ -3242,11 +3300,11 @@
         <v>22068.454545454544</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1277668</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>675512.12168109661</v>
       </c>
       <c r="V55" s="1">
@@ -3273,11 +3331,11 @@
         <v>24809.363636363636</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1370228</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>700321.48531746026</v>
       </c>
       <c r="V56" s="1">
@@ -3304,11 +3362,11 @@
         <v>28342.545454545456</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1440848</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>728664.03077200567</v>
       </c>
       <c r="V57" s="1">
@@ -3335,11 +3393,11 @@
         <v>26309.272727272728</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1497008</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>754973.30349927838</v>
       </c>
       <c r="V58" s="1">
@@ -3366,11 +3424,11 @@
         <v>23571.727272727272</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1540279</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>778545.03077200567</v>
       </c>
       <c r="V59" s="1">
@@ -3397,11 +3455,11 @@
         <v>21629.454545454544</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1594464</v>
       </c>
       <c r="U60" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>800174.48531746026</v>
       </c>
       <c r="V60" s="1">
@@ -3428,11 +3486,11 @@
         <v>21511.909090909092</v>
       </c>
       <c r="T61" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1642593</v>
       </c>
       <c r="U61" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>821686.39440836932</v>
       </c>
       <c r="V61" s="1">
@@ -3459,11 +3517,11 @@
         <v>19461.272727272728</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1678981</v>
       </c>
       <c r="U62" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>841147.66713564203</v>
       </c>
       <c r="V62" s="1">
@@ -3490,11 +3548,11 @@
         <v>17916.636363636364</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1711287</v>
       </c>
       <c r="U63" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>859064.30349927838</v>
       </c>
       <c r="V63" s="1">
@@ -3521,11 +3579,11 @@
         <v>17763.909090909092</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1744119</v>
       </c>
       <c r="U64" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>876828.21259018744</v>
       </c>
       <c r="V64" s="1">
@@ -3552,11 +3610,11 @@
         <v>17535.090909090908</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1768866</v>
       </c>
       <c r="U65" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>894363.30349927838</v>
       </c>
       <c r="V65" s="1">
@@ -3583,11 +3641,11 @@
         <v>17130.18181818182</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1794920</v>
       </c>
       <c r="U66" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>911493.48531746014</v>
       </c>
       <c r="V66" s="1">
@@ -3614,11 +3672,11 @@
         <v>17186.363636363636</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>1816116</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>928679.84895382379</v>
       </c>
       <c r="V67" s="1">
@@ -3645,11 +3703,11 @@
         <v>14679.636363636364</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" ref="T68:U83" si="23">T67+R68</f>
+        <f t="shared" ref="T68:U83" si="29">T67+R68</f>
         <v>1846521</v>
       </c>
       <c r="U68" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>943359.48531746014</v>
       </c>
       <c r="V68" s="1">
@@ -3676,11 +3734,11 @@
         <v>15690.818181818182</v>
       </c>
       <c r="T69" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1878833</v>
       </c>
       <c r="U69" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>959050.30349927838</v>
       </c>
       <c r="V69" s="1">
@@ -3707,11 +3765,11 @@
         <v>14967.545454545454</v>
       </c>
       <c r="T70" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1901010</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>974017.84895382379</v>
       </c>
       <c r="V70" s="1">
@@ -3738,11 +3796,11 @@
         <v>14546.818181818182</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1914981</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>988564.66713564203</v>
       </c>
       <c r="V71" s="1">
@@ -3769,11 +3827,11 @@
         <v>13876.272727272728</v>
       </c>
       <c r="T72" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1928616</v>
       </c>
       <c r="U72" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1002440.9398629147</v>
       </c>
       <c r="V72" s="1">
@@ -3800,11 +3858,11 @@
         <v>12522.363636363636</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1938412</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1014963.3034992784</v>
       </c>
       <c r="V73" s="1">
@@ -3831,11 +3889,11 @@
         <v>12105.636363636364</v>
       </c>
       <c r="T74" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1946010</v>
       </c>
       <c r="U74" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1027068.9398629147</v>
       </c>
       <c r="V74" s="1">
@@ -3862,11 +3920,11 @@
         <v>11272.545454545454</v>
       </c>
       <c r="T75" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1953188</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1038341.4853174601</v>
       </c>
       <c r="V75" s="1">
@@ -3893,11 +3951,11 @@
         <v>9771.0909090909099</v>
       </c>
       <c r="T76" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1962346</v>
       </c>
       <c r="U76" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1048112.5762265511</v>
       </c>
       <c r="V76" s="1">
@@ -3924,11 +3982,11 @@
         <v>7589.909090909091</v>
       </c>
       <c r="T77" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1973666</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1055702.4853174603</v>
       </c>
       <c r="V77" s="1">
@@ -3955,11 +4013,11 @@
         <v>8318.545454545454</v>
       </c>
       <c r="T78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1981697</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1064021.0307720057</v>
       </c>
       <c r="V78" s="1">
@@ -3986,11 +4044,11 @@
         <v>7405.727272727273</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1991144</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1071426.758044733</v>
       </c>
       <c r="V79" s="1">
@@ -4017,11 +4075,11 @@
         <v>7004.181818181818</v>
       </c>
       <c r="T80" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>2001289</v>
       </c>
       <c r="U80" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1078430.9398629148</v>
       </c>
       <c r="V80" s="1">
@@ -4048,11 +4106,11 @@
         <v>6677.818181818182</v>
       </c>
       <c r="T81" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>2013289</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1085108.758044733</v>
       </c>
       <c r="V81" s="1">
@@ -4079,11 +4137,11 @@
         <v>6140.454545454545</v>
       </c>
       <c r="T82" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>2026172</v>
       </c>
       <c r="U82" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1091249.2125901876</v>
       </c>
       <c r="V82" s="1">
@@ -4110,11 +4168,11 @@
         <v>6411.4</v>
       </c>
       <c r="T83" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>2032538</v>
       </c>
       <c r="U83" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>1097660.6125901875</v>
       </c>
       <c r="V83" s="1">
@@ -4141,11 +4199,11 @@
         <v>6189.6</v>
       </c>
       <c r="T84" s="1">
-        <f t="shared" ref="T84:U99" si="24">T83+R84</f>
+        <f t="shared" ref="T84:U99" si="30">T83+R84</f>
         <v>2036693</v>
       </c>
       <c r="U84" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1103850.2125901876</v>
       </c>
       <c r="V84" s="1">
@@ -4172,11 +4230,11 @@
         <v>4314.3999999999996</v>
       </c>
       <c r="T85" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2039343</v>
       </c>
       <c r="U85" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1108164.6125901875</v>
       </c>
       <c r="V85" s="1">
@@ -4203,11 +4261,11 @@
         <v>3802.6</v>
       </c>
       <c r="T86" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2043072</v>
       </c>
       <c r="U86" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1111967.2125901876</v>
       </c>
       <c r="V86" s="1">
@@ -4234,11 +4292,11 @@
         <v>3261.3333333333335</v>
       </c>
       <c r="T87" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2045727</v>
       </c>
       <c r="U87" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1115228.5459235208</v>
       </c>
       <c r="V87" s="1">
@@ -4265,11 +4323,11 @@
         <v>2728.4444444444443</v>
       </c>
       <c r="T88" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2047725</v>
       </c>
       <c r="U88" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1117956.9903679653</v>
       </c>
       <c r="V88" s="1">
@@ -4296,11 +4354,11 @@
         <v>2059.7777777777778</v>
       </c>
       <c r="T89" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2049017</v>
       </c>
       <c r="U89" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1120016.7681457431</v>
       </c>
       <c r="V89" s="1">
@@ -4327,11 +4385,11 @@
         <v>1764.2222222222222</v>
       </c>
       <c r="T90" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2049846</v>
       </c>
       <c r="U90" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1121780.9903679653</v>
       </c>
       <c r="V90" s="1">
@@ -4358,11 +4416,11 @@
         <v>1664.125</v>
       </c>
       <c r="T91" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2051014</v>
       </c>
       <c r="U91" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1123445.1153679653</v>
       </c>
       <c r="V91" s="1">
@@ -4389,11 +4447,11 @@
         <v>1687.375</v>
       </c>
       <c r="T92" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2051949</v>
       </c>
       <c r="U92" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1125132.4903679653</v>
       </c>
       <c r="V92" s="1">
@@ -4420,11 +4478,11 @@
         <v>868.83333333333337</v>
       </c>
       <c r="T93" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U93" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1126001.3237012986</v>
       </c>
       <c r="V93" s="1">
@@ -4448,11 +4506,11 @@
         <v>707.66666666666663</v>
       </c>
       <c r="T94" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U94" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1126708.9903679653</v>
       </c>
       <c r="V94" s="1">
@@ -4476,11 +4534,11 @@
         <v>440</v>
       </c>
       <c r="T95" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U95" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1127148.9903679653</v>
       </c>
       <c r="V95" s="1">
@@ -4504,11 +4562,11 @@
         <v>720.66666666666663</v>
       </c>
       <c r="T96" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U96" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1127869.6570346321</v>
       </c>
       <c r="V96" s="1">
@@ -4532,11 +4590,11 @@
         <v>238</v>
       </c>
       <c r="T97" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U97" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1128107.6570346321</v>
       </c>
       <c r="V97" s="1">
@@ -4560,11 +4618,11 @@
         <v>323</v>
       </c>
       <c r="T98" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U98" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1128430.6570346321</v>
       </c>
       <c r="V98" s="1">
@@ -4588,11 +4646,11 @@
         <v>250</v>
       </c>
       <c r="T99" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>2052845</v>
       </c>
       <c r="U99" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V99" s="1">
@@ -4613,11 +4671,11 @@
         <v>45572</v>
       </c>
       <c r="T100" s="1">
-        <f t="shared" ref="T100:U108" si="25">T99+R100</f>
+        <f t="shared" ref="T100:U108" si="31">T99+R100</f>
         <v>2052845</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V100" s="1">
@@ -4638,11 +4696,11 @@
         <v>45573</v>
       </c>
       <c r="T101" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V101" s="1">
@@ -4657,11 +4715,11 @@
         <v>45574</v>
       </c>
       <c r="T102" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V102" s="1">
@@ -4676,11 +4734,11 @@
         <v>45575</v>
       </c>
       <c r="T103" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V103" s="1">
@@ -4695,11 +4753,11 @@
         <v>45576</v>
       </c>
       <c r="T104" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V104" s="1">
@@ -4714,11 +4772,11 @@
         <v>45577</v>
       </c>
       <c r="T105" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V105" s="1">
@@ -4733,11 +4791,11 @@
         <v>45578</v>
       </c>
       <c r="T106" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V106" s="1">
@@ -4752,11 +4810,11 @@
         <v>45579</v>
       </c>
       <c r="T107" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V107" s="1">
@@ -4771,11 +4829,11 @@
         <v>45580</v>
       </c>
       <c r="T108" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>2052845</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V108" s="1">

</xml_diff>

<commit_message>
aug 2 update 4 appendix a
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1E7C0DA-7D5E-417D-B7C4-FCCD100A5DD7}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2628363-1FCE-4278-94DA-F81E9CBB2179}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="4510" yWindow="1630" windowWidth="16800" windowHeight="11350" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30:Q32"/>
+      <selection pane="bottomRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2715,11 +2715,11 @@
         <v>140075</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" ref="M30:M32" si="38">I30+K30</f>
+        <f t="shared" ref="M30" si="38">I30+K30</f>
         <v>0</v>
       </c>
       <c r="N30" s="2">
-        <f t="shared" ref="N30:N32" si="39">B30+M30</f>
+        <f t="shared" ref="N30" si="39">B30+M30</f>
         <v>14197</v>
       </c>
       <c r="O30" s="1">
@@ -2727,7 +2727,7 @@
         <v>140075</v>
       </c>
       <c r="P30" s="1">
-        <f t="shared" ref="P30:P32" si="41">C30+J30</f>
+        <f t="shared" ref="P30" si="41">C30+J30</f>
         <v>1005</v>
       </c>
       <c r="Q30" s="1">
@@ -2800,11 +2800,11 @@
         <v>149686</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" ref="M31:M32" si="44">I31+K31</f>
+        <f t="shared" ref="M31:M33" si="44">I31+K31</f>
         <v>0</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" ref="N31:N32" si="45">B31+M31</f>
+        <f t="shared" ref="N31:N33" si="45">B31+M31</f>
         <v>9611</v>
       </c>
       <c r="O31" s="1">
@@ -2812,7 +2812,7 @@
         <v>149686</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" ref="P31:P32" si="47">C31+J31</f>
+        <f t="shared" ref="P31:P33" si="47">C31+J31</f>
         <v>705</v>
       </c>
       <c r="Q31" s="1">
@@ -2935,6 +2935,60 @@
       <c r="A33" s="3">
         <v>45505</v>
       </c>
+      <c r="B33">
+        <v>17509</v>
+      </c>
+      <c r="C33">
+        <v>1417</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>57</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <f t="shared" ref="L33" si="49">L32+B33</f>
+        <v>177251</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" ref="M33" si="50">I33+K33</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" ref="N33" si="51">B33+M33</f>
+        <v>17509</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" ref="O33" si="52">O32+N33</f>
+        <v>177251</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" ref="P33" si="53">C33+J33</f>
+        <v>1417</v>
+      </c>
+      <c r="Q33" s="1">
+        <f t="shared" ref="Q33" si="54">P33+Q32</f>
+        <v>10250</v>
+      </c>
       <c r="R33" s="1">
         <v>21710</v>
       </c>
@@ -3035,11 +3089,11 @@
         <v>18790.8</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" ref="T36:U51" si="49">T35+R36</f>
+        <f t="shared" ref="T36:U51" si="55">T35+R36</f>
         <v>520442</v>
       </c>
       <c r="U36" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>179104.5853174603</v>
       </c>
       <c r="V36" s="1">
@@ -3066,11 +3120,11 @@
         <v>25713.3</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>550390</v>
       </c>
       <c r="U37" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>204817.88531746028</v>
       </c>
       <c r="V37" s="1">
@@ -3097,11 +3151,11 @@
         <v>18006.400000000001</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>581098</v>
       </c>
       <c r="U38" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>222824.28531746028</v>
       </c>
       <c r="V38" s="1">
@@ -3128,11 +3182,11 @@
         <v>24560.3</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>605588</v>
       </c>
       <c r="U39" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>247384.58531746027</v>
       </c>
       <c r="V39" s="1">
@@ -3159,11 +3213,11 @@
         <v>22302.5</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>627171</v>
       </c>
       <c r="U40" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>269687.08531746024</v>
       </c>
       <c r="V40" s="1">
@@ -3190,11 +3244,11 @@
         <v>36342.400000000001</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>652373</v>
       </c>
       <c r="U41" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>306029.48531746026</v>
       </c>
       <c r="V41" s="1">
@@ -3221,11 +3275,11 @@
         <v>26445.363636363636</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>675506</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>332474.84895382391</v>
       </c>
       <c r="V42" s="1">
@@ -3252,11 +3306,11 @@
         <v>28798.363636363636</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>717110</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>361273.21259018756</v>
       </c>
       <c r="V43" s="1">
@@ -3283,11 +3337,11 @@
         <v>22717.545454545456</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>740207</v>
       </c>
       <c r="U44" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>383990.75804473303</v>
       </c>
       <c r="V44" s="1">
@@ -3314,11 +3368,11 @@
         <v>24761.090909090908</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>770155</v>
       </c>
       <c r="U45" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>408751.84895382391</v>
       </c>
       <c r="V45" s="1">
@@ -3345,11 +3399,11 @@
         <v>27668.909090909092</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>813557</v>
       </c>
       <c r="U46" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>436420.75804473303</v>
       </c>
       <c r="V46" s="1">
@@ -3376,11 +3430,11 @@
         <v>28715</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>849071</v>
       </c>
       <c r="U47" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>465135.75804473303</v>
       </c>
       <c r="V47" s="1">
@@ -3407,11 +3461,11 @@
         <v>19741.18181818182</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>891191</v>
       </c>
       <c r="U48" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>484876.93986291485</v>
       </c>
       <c r="V48" s="1">
@@ -3438,11 +3492,11 @@
         <v>24994.81818181818</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>963510</v>
       </c>
       <c r="U49" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>509871.75804473303</v>
       </c>
       <c r="V49" s="1">
@@ -3469,11 +3523,11 @@
         <v>30512.18181818182</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1014593</v>
       </c>
       <c r="U50" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>540383.93986291485</v>
       </c>
       <c r="V50" s="1">
@@ -3500,11 +3554,11 @@
         <v>29755.272727272728</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>1077884</v>
       </c>
       <c r="U51" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="55"/>
         <v>570139.21259018756</v>
       </c>
       <c r="V51" s="1">
@@ -3531,11 +3585,11 @@
         <v>29568.909090909092</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" ref="T52:U67" si="50">T51+R52</f>
+        <f t="shared" ref="T52:U67" si="56">T51+R52</f>
         <v>1114483</v>
       </c>
       <c r="U52" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>599708.12168109661</v>
       </c>
       <c r="V52" s="1">
@@ -3562,11 +3616,11 @@
         <v>27004.636363636364</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1174452</v>
       </c>
       <c r="U53" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>626712.75804473297</v>
       </c>
       <c r="V53" s="1">
@@ -3593,11 +3647,11 @@
         <v>26730.909090909092</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1202504</v>
       </c>
       <c r="U54" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>653443.66713564203</v>
       </c>
       <c r="V54" s="1">
@@ -3624,11 +3678,11 @@
         <v>22068.454545454544</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1277668</v>
       </c>
       <c r="U55" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>675512.12168109661</v>
       </c>
       <c r="V55" s="1">
@@ -3655,11 +3709,11 @@
         <v>24809.363636363636</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1370228</v>
       </c>
       <c r="U56" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>700321.48531746026</v>
       </c>
       <c r="V56" s="1">
@@ -3686,11 +3740,11 @@
         <v>28342.545454545456</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1440848</v>
       </c>
       <c r="U57" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>728664.03077200567</v>
       </c>
       <c r="V57" s="1">
@@ -3717,11 +3771,11 @@
         <v>26309.272727272728</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1497008</v>
       </c>
       <c r="U58" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>754973.30349927838</v>
       </c>
       <c r="V58" s="1">
@@ -3748,11 +3802,11 @@
         <v>23571.727272727272</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1540279</v>
       </c>
       <c r="U59" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>778545.03077200567</v>
       </c>
       <c r="V59" s="1">
@@ -3779,11 +3833,11 @@
         <v>21629.454545454544</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1594464</v>
       </c>
       <c r="U60" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>800174.48531746026</v>
       </c>
       <c r="V60" s="1">
@@ -3810,11 +3864,11 @@
         <v>21511.909090909092</v>
       </c>
       <c r="T61" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1642593</v>
       </c>
       <c r="U61" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>821686.39440836932</v>
       </c>
       <c r="V61" s="1">
@@ -3841,11 +3895,11 @@
         <v>19461.272727272728</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1678981</v>
       </c>
       <c r="U62" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>841147.66713564203</v>
       </c>
       <c r="V62" s="1">
@@ -3872,11 +3926,11 @@
         <v>17916.636363636364</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1711287</v>
       </c>
       <c r="U63" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>859064.30349927838</v>
       </c>
       <c r="V63" s="1">
@@ -3903,11 +3957,11 @@
         <v>17763.909090909092</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1744119</v>
       </c>
       <c r="U64" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>876828.21259018744</v>
       </c>
       <c r="V64" s="1">
@@ -3934,11 +3988,11 @@
         <v>17535.090909090908</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1768866</v>
       </c>
       <c r="U65" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>894363.30349927838</v>
       </c>
       <c r="V65" s="1">
@@ -3965,11 +4019,11 @@
         <v>17130.18181818182</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1794920</v>
       </c>
       <c r="U66" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>911493.48531746014</v>
       </c>
       <c r="V66" s="1">
@@ -3996,11 +4050,11 @@
         <v>17186.363636363636</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>1816116</v>
       </c>
       <c r="U67" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="56"/>
         <v>928679.84895382379</v>
       </c>
       <c r="V67" s="1">
@@ -4027,11 +4081,11 @@
         <v>14679.636363636364</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" ref="T68:U83" si="51">T67+R68</f>
+        <f t="shared" ref="T68:U83" si="57">T67+R68</f>
         <v>1846521</v>
       </c>
       <c r="U68" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>943359.48531746014</v>
       </c>
       <c r="V68" s="1">
@@ -4058,11 +4112,11 @@
         <v>15690.818181818182</v>
       </c>
       <c r="T69" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1878833</v>
       </c>
       <c r="U69" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>959050.30349927838</v>
       </c>
       <c r="V69" s="1">
@@ -4089,11 +4143,11 @@
         <v>14967.545454545454</v>
       </c>
       <c r="T70" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1901010</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>974017.84895382379</v>
       </c>
       <c r="V70" s="1">
@@ -4120,11 +4174,11 @@
         <v>14546.818181818182</v>
       </c>
       <c r="T71" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1914981</v>
       </c>
       <c r="U71" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>988564.66713564203</v>
       </c>
       <c r="V71" s="1">
@@ -4151,11 +4205,11 @@
         <v>13876.272727272728</v>
       </c>
       <c r="T72" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1928616</v>
       </c>
       <c r="U72" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1002440.9398629147</v>
       </c>
       <c r="V72" s="1">
@@ -4182,11 +4236,11 @@
         <v>12522.363636363636</v>
       </c>
       <c r="T73" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1938412</v>
       </c>
       <c r="U73" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1014963.3034992784</v>
       </c>
       <c r="V73" s="1">
@@ -4213,11 +4267,11 @@
         <v>12105.636363636364</v>
       </c>
       <c r="T74" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1946010</v>
       </c>
       <c r="U74" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1027068.9398629147</v>
       </c>
       <c r="V74" s="1">
@@ -4244,11 +4298,11 @@
         <v>11272.545454545454</v>
       </c>
       <c r="T75" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1953188</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1038341.4853174601</v>
       </c>
       <c r="V75" s="1">
@@ -4275,11 +4329,11 @@
         <v>9771.0909090909099</v>
       </c>
       <c r="T76" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1962346</v>
       </c>
       <c r="U76" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1048112.5762265511</v>
       </c>
       <c r="V76" s="1">
@@ -4306,11 +4360,11 @@
         <v>7589.909090909091</v>
       </c>
       <c r="T77" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1973666</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1055702.4853174603</v>
       </c>
       <c r="V77" s="1">
@@ -4337,11 +4391,11 @@
         <v>8318.545454545454</v>
       </c>
       <c r="T78" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1981697</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1064021.0307720057</v>
       </c>
       <c r="V78" s="1">
@@ -4368,11 +4422,11 @@
         <v>7405.727272727273</v>
       </c>
       <c r="T79" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1991144</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1071426.758044733</v>
       </c>
       <c r="V79" s="1">
@@ -4399,11 +4453,11 @@
         <v>7004.181818181818</v>
       </c>
       <c r="T80" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2001289</v>
       </c>
       <c r="U80" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1078430.9398629148</v>
       </c>
       <c r="V80" s="1">
@@ -4430,11 +4484,11 @@
         <v>6677.818181818182</v>
       </c>
       <c r="T81" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2013289</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1085108.758044733</v>
       </c>
       <c r="V81" s="1">
@@ -4461,11 +4515,11 @@
         <v>6140.454545454545</v>
       </c>
       <c r="T82" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2026172</v>
       </c>
       <c r="U82" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1091249.2125901876</v>
       </c>
       <c r="V82" s="1">
@@ -4492,11 +4546,11 @@
         <v>6411.4</v>
       </c>
       <c r="T83" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>2032538</v>
       </c>
       <c r="U83" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="57"/>
         <v>1097660.6125901875</v>
       </c>
       <c r="V83" s="1">
@@ -4523,11 +4577,11 @@
         <v>6189.6</v>
       </c>
       <c r="T84" s="1">
-        <f t="shared" ref="T84:U99" si="52">T83+R84</f>
+        <f t="shared" ref="T84:U99" si="58">T83+R84</f>
         <v>2036693</v>
       </c>
       <c r="U84" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1103850.2125901876</v>
       </c>
       <c r="V84" s="1">
@@ -4554,11 +4608,11 @@
         <v>4314.3999999999996</v>
       </c>
       <c r="T85" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2039343</v>
       </c>
       <c r="U85" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1108164.6125901875</v>
       </c>
       <c r="V85" s="1">
@@ -4585,11 +4639,11 @@
         <v>3802.6</v>
       </c>
       <c r="T86" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2043072</v>
       </c>
       <c r="U86" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1111967.2125901876</v>
       </c>
       <c r="V86" s="1">
@@ -4616,11 +4670,11 @@
         <v>3261.3333333333335</v>
       </c>
       <c r="T87" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2045727</v>
       </c>
       <c r="U87" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1115228.5459235208</v>
       </c>
       <c r="V87" s="1">
@@ -4647,11 +4701,11 @@
         <v>2728.4444444444443</v>
       </c>
       <c r="T88" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2047725</v>
       </c>
       <c r="U88" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1117956.9903679653</v>
       </c>
       <c r="V88" s="1">
@@ -4678,11 +4732,11 @@
         <v>2059.7777777777778</v>
       </c>
       <c r="T89" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2049017</v>
       </c>
       <c r="U89" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1120016.7681457431</v>
       </c>
       <c r="V89" s="1">
@@ -4709,11 +4763,11 @@
         <v>1764.2222222222222</v>
       </c>
       <c r="T90" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2049846</v>
       </c>
       <c r="U90" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1121780.9903679653</v>
       </c>
       <c r="V90" s="1">
@@ -4740,11 +4794,11 @@
         <v>1664.125</v>
       </c>
       <c r="T91" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2051014</v>
       </c>
       <c r="U91" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1123445.1153679653</v>
       </c>
       <c r="V91" s="1">
@@ -4771,11 +4825,11 @@
         <v>1687.375</v>
       </c>
       <c r="T92" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2051949</v>
       </c>
       <c r="U92" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1125132.4903679653</v>
       </c>
       <c r="V92" s="1">
@@ -4802,11 +4856,11 @@
         <v>868.83333333333337</v>
       </c>
       <c r="T93" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U93" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1126001.3237012986</v>
       </c>
       <c r="V93" s="1">
@@ -4830,11 +4884,11 @@
         <v>707.66666666666663</v>
       </c>
       <c r="T94" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U94" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1126708.9903679653</v>
       </c>
       <c r="V94" s="1">
@@ -4858,11 +4912,11 @@
         <v>440</v>
       </c>
       <c r="T95" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U95" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1127148.9903679653</v>
       </c>
       <c r="V95" s="1">
@@ -4886,11 +4940,11 @@
         <v>720.66666666666663</v>
       </c>
       <c r="T96" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U96" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1127869.6570346321</v>
       </c>
       <c r="V96" s="1">
@@ -4914,11 +4968,11 @@
         <v>238</v>
       </c>
       <c r="T97" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U97" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1128107.6570346321</v>
       </c>
       <c r="V97" s="1">
@@ -4942,11 +4996,11 @@
         <v>323</v>
       </c>
       <c r="T98" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U98" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1128430.6570346321</v>
       </c>
       <c r="V98" s="1">
@@ -4970,11 +5024,11 @@
         <v>250</v>
       </c>
       <c r="T99" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>2052845</v>
       </c>
       <c r="U99" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="58"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V99" s="1">
@@ -4995,11 +5049,11 @@
         <v>45572</v>
       </c>
       <c r="T100" s="1">
-        <f t="shared" ref="T100:U108" si="53">T99+R100</f>
+        <f t="shared" ref="T100:U108" si="59">T99+R100</f>
         <v>2052845</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V100" s="1">
@@ -5020,11 +5074,11 @@
         <v>45573</v>
       </c>
       <c r="T101" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V101" s="1">
@@ -5039,11 +5093,11 @@
         <v>45574</v>
       </c>
       <c r="T102" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V102" s="1">
@@ -5058,11 +5112,11 @@
         <v>45575</v>
       </c>
       <c r="T103" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V103" s="1">
@@ -5077,11 +5131,11 @@
         <v>45576</v>
       </c>
       <c r="T104" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V104" s="1">
@@ -5096,11 +5150,11 @@
         <v>45577</v>
       </c>
       <c r="T105" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V105" s="1">
@@ -5115,11 +5169,11 @@
         <v>45578</v>
       </c>
       <c r="T106" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V106" s="1">
@@ -5134,11 +5188,11 @@
         <v>45579</v>
       </c>
       <c r="T107" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V107" s="1">
@@ -5153,11 +5207,11 @@
         <v>45580</v>
       </c>
       <c r="T108" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>2052845</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="53"/>
+        <f t="shared" si="59"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="V108" s="1">

</xml_diff>

<commit_message>
update babine data 8/17
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{5002ADF5-552C-4695-A0BF-EDC672F0F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{481AA086-9072-4EDA-89C2-7099B0FEAC3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB783FD0-04CC-154B-B164-FDD0C1903F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="70" windowWidth="16270" windowHeight="11900" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="5480" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -178,10 +178,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,30 +500,30 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K51" sqref="K51"/>
+      <selection pane="bottomRight" activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="1"/>
-    <col min="15" max="15" width="8.7265625" style="2"/>
-    <col min="16" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="17" width="13.6328125" style="1" customWidth="1"/>
-    <col min="18" max="23" width="8.7265625" style="1"/>
-    <col min="24" max="24" width="9.7265625" style="1" customWidth="1"/>
-    <col min="25" max="26" width="11.7265625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="1"/>
+    <col min="15" max="15" width="8.6640625" style="2"/>
+    <col min="16" max="16" width="8.6640625" style="1"/>
+    <col min="17" max="17" width="13.6640625" style="1" customWidth="1"/>
+    <col min="18" max="23" width="8.6640625" style="1"/>
+    <col min="24" max="24" width="9.6640625" style="1" customWidth="1"/>
+    <col min="25" max="26" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +603,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45474</v>
       </c>
@@ -654,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45475</v>
       </c>
@@ -701,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45476</v>
       </c>
@@ -748,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45477</v>
       </c>
@@ -795,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>45478</v>
       </c>
@@ -842,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>45479</v>
       </c>
@@ -889,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>45480</v>
       </c>
@@ -936,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>45481</v>
       </c>
@@ -983,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>45482</v>
       </c>
@@ -1071,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>45483</v>
       </c>
@@ -1159,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>45484</v>
       </c>
@@ -1247,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>45485</v>
       </c>
@@ -1335,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>45486</v>
       </c>
@@ -1423,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>45487</v>
       </c>
@@ -1511,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>45488</v>
       </c>
@@ -1599,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>45489</v>
       </c>
@@ -1687,7 +1683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>45490</v>
       </c>
@@ -1775,7 +1771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>45491</v>
       </c>
@@ -1863,7 +1859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>45492</v>
       </c>
@@ -1951,7 +1947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>45493</v>
       </c>
@@ -2039,7 +2035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>45494</v>
       </c>
@@ -2127,7 +2123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>45495</v>
       </c>
@@ -2215,7 +2211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>45496</v>
       </c>
@@ -2303,7 +2299,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>45497</v>
       </c>
@@ -2391,7 +2387,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>45498</v>
       </c>
@@ -2479,7 +2475,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>45499</v>
       </c>
@@ -2567,7 +2563,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>45500</v>
       </c>
@@ -2655,7 +2651,7 @@
         <v>5397</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>45501</v>
       </c>
@@ -2743,7 +2739,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>45502</v>
       </c>
@@ -2831,7 +2827,7 @@
         <v>28914</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>45503</v>
       </c>
@@ -2919,7 +2915,7 @@
         <v>78670</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>45504</v>
       </c>
@@ -3007,7 +3003,7 @@
         <v>95995</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>45505</v>
       </c>
@@ -3095,7 +3091,7 @@
         <v>114013</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>45506</v>
       </c>
@@ -3183,7 +3179,7 @@
         <v>89321</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>45507</v>
       </c>
@@ -3271,7 +3267,7 @@
         <v>56123</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>45508</v>
       </c>
@@ -3359,7 +3355,7 @@
         <v>52046</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>45509</v>
       </c>
@@ -3447,7 +3443,7 @@
         <v>71155</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>45510</v>
       </c>
@@ -3535,7 +3531,7 @@
         <v>72186</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>45511</v>
       </c>
@@ -3623,7 +3619,7 @@
         <v>62076</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>45512</v>
       </c>
@@ -3711,7 +3707,7 @@
         <v>49081</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>45513</v>
       </c>
@@ -3799,7 +3795,7 @@
         <v>66336</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>45514</v>
       </c>
@@ -3887,7 +3883,7 @@
         <v>68262</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>45515</v>
       </c>
@@ -3975,7 +3971,7 @@
         <v>78487</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>45516</v>
       </c>
@@ -4063,7 +4059,7 @@
         <v>86699</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>45517</v>
       </c>
@@ -4151,7 +4147,7 @@
         <v>77654</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45518</v>
       </c>
@@ -4193,7 +4189,7 @@
         <v>917980</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" ref="N46:N48" si="79">J46+L46</f>
+        <f t="shared" ref="N46" si="79">J46+L46</f>
         <v>0</v>
       </c>
       <c r="O46" s="2">
@@ -4205,7 +4201,7 @@
         <v>918212</v>
       </c>
       <c r="Q46" s="1">
-        <f t="shared" ref="Q46:Q48" si="81">C46+K46</f>
+        <f t="shared" ref="Q46" si="81">C46+K46</f>
         <v>5760</v>
       </c>
       <c r="R46" s="1">
@@ -4239,7 +4235,7 @@
         <v>96699</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>45519</v>
       </c>
@@ -4277,27 +4273,27 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47:M48" si="83">M46+B47</f>
+        <f t="shared" ref="M47:M49" si="83">M46+B47</f>
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N48" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N49" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O48" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O49" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P48" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P49" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q48" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q49" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R48" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R49" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -4327,7 +4323,7 @@
         <v>97035</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>45520</v>
       </c>
@@ -4415,9 +4411,66 @@
         <v>101868</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>45521</v>
+      </c>
+      <c r="B49">
+        <v>95923</v>
+      </c>
+      <c r="C49">
+        <v>3645</v>
+      </c>
+      <c r="D49">
+        <v>12</v>
+      </c>
+      <c r="E49">
+        <v>12428</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>29</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1">
+        <f t="shared" si="83"/>
+        <v>1156839</v>
+      </c>
+      <c r="N49" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="85"/>
+        <v>95952</v>
+      </c>
+      <c r="P49" s="1">
+        <f t="shared" si="86"/>
+        <v>1157168</v>
+      </c>
+      <c r="Q49" s="1">
+        <f t="shared" si="87"/>
+        <v>3645</v>
+      </c>
+      <c r="R49" s="1">
+        <f t="shared" si="88"/>
+        <v>65725</v>
       </c>
       <c r="S49" s="1">
         <v>72319</v>
@@ -4446,7 +4499,7 @@
         <v>95563</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>45522</v>
       </c>
@@ -4477,7 +4530,7 @@
         <v>96290</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>45523</v>
       </c>
@@ -4508,7 +4561,7 @@
         <v>76587</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>45524</v>
       </c>
@@ -4539,7 +4592,7 @@
         <v>69901</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>45525</v>
       </c>
@@ -4570,7 +4623,7 @@
         <v>76507</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>45526</v>
       </c>
@@ -4601,7 +4654,7 @@
         <v>98879</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>45527</v>
       </c>
@@ -4632,7 +4685,7 @@
         <v>95316</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>45528</v>
       </c>
@@ -4663,7 +4716,7 @@
         <v>83573</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>45529</v>
       </c>
@@ -4694,7 +4747,7 @@
         <v>94051</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>45530</v>
       </c>
@@ -4725,7 +4778,7 @@
         <v>89303</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>45531</v>
       </c>
@@ -4756,7 +4809,7 @@
         <v>58380</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>45532</v>
       </c>
@@ -4787,7 +4840,7 @@
         <v>65722</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>45533</v>
       </c>
@@ -4818,7 +4871,7 @@
         <v>54403</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>45534</v>
       </c>
@@ -4849,7 +4902,7 @@
         <v>47793</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>45535</v>
       </c>
@@ -4880,7 +4933,7 @@
         <v>35932</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>45536</v>
       </c>
@@ -4911,7 +4964,7 @@
         <v>28559</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>45537</v>
       </c>
@@ -4942,7 +4995,7 @@
         <v>22150</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>45538</v>
       </c>
@@ -4973,7 +5026,7 @@
         <v>20493</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>45539</v>
       </c>
@@ -5004,7 +5057,7 @@
         <v>20387</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>45540</v>
       </c>
@@ -5035,7 +5088,7 @@
         <v>37971</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>45541</v>
       </c>
@@ -5066,7 +5119,7 @@
         <v>31544</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>45542</v>
       </c>
@@ -5097,7 +5150,7 @@
         <v>21102</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>45543</v>
       </c>
@@ -5128,7 +5181,7 @@
         <v>16385</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>45544</v>
       </c>
@@ -5159,7 +5212,7 @@
         <v>16372</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>45545</v>
       </c>
@@ -5190,7 +5243,7 @@
         <v>16658</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>45546</v>
       </c>
@@ -5221,7 +5274,7 @@
         <v>12902</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>45547</v>
       </c>
@@ -5252,7 +5305,7 @@
         <v>12105</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>45548</v>
       </c>
@@ -5283,7 +5336,7 @@
         <v>10400</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>45549</v>
       </c>
@@ -5314,7 +5367,7 @@
         <v>10842</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>45550</v>
       </c>
@@ -5345,7 +5398,7 @@
         <v>8295</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>45551</v>
       </c>
@@ -5376,7 +5429,7 @@
         <v>7467</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>45552</v>
       </c>
@@ -5407,7 +5460,7 @@
         <v>6134</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>45553</v>
       </c>
@@ -5438,7 +5491,7 @@
         <v>6635</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>45554</v>
       </c>
@@ -5469,7 +5522,7 @@
         <v>6004</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>45555</v>
       </c>
@@ -5500,7 +5553,7 @@
         <v>4777</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>45556</v>
       </c>
@@ -5531,7 +5584,7 @@
         <v>4552</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>45557</v>
       </c>
@@ -5562,7 +5615,7 @@
         <v>3637</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>45558</v>
       </c>
@@ -5593,7 +5646,7 @@
         <v>2859</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>45559</v>
       </c>
@@ -5624,7 +5677,7 @@
         <v>2617</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>45560</v>
       </c>
@@ -5655,7 +5708,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>45561</v>
       </c>
@@ -5686,7 +5739,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>45562</v>
       </c>
@@ -5717,7 +5770,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>45563</v>
       </c>
@@ -5748,7 +5801,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>45564</v>
       </c>
@@ -5779,7 +5832,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>45565</v>
       </c>
@@ -5810,7 +5863,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>45566</v>
       </c>
@@ -5838,7 +5891,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>45567</v>
       </c>
@@ -5866,7 +5919,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>45568</v>
       </c>
@@ -5894,7 +5947,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>45569</v>
       </c>
@@ -5922,7 +5975,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>45570</v>
       </c>
@@ -5950,7 +6003,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>45571</v>
       </c>
@@ -5978,7 +6031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>45572</v>
       </c>
@@ -6003,7 +6056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>45573</v>
       </c>
@@ -6022,7 +6075,7 @@
         <v>110480.125</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>45574</v>
       </c>
@@ -6041,7 +6094,7 @@
         <v>110489.25</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>45575</v>
       </c>
@@ -6060,7 +6113,7 @@
         <v>110499.3125</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>45576</v>
       </c>
@@ -6079,7 +6132,7 @@
         <v>110509.28125</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>45577</v>
       </c>
@@ -6098,7 +6151,7 @@
         <v>110512.625</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>45578</v>
       </c>
@@ -6117,7 +6170,7 @@
         <v>110516.34375</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>45579</v>
       </c>
@@ -6136,7 +6189,7 @@
         <v>110519.1875</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>45580</v>
       </c>

</xml_diff>

<commit_message>
8/19/24 Tyee and Babine updates
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB783FD0-04CC-154B-B164-FDD0C1903F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C691AF-5C63-E240-93CA-EA47D1259FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="6300" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S45" sqref="S45"/>
+      <selection pane="bottomRight" activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4273,27 +4273,27 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47:M49" si="83">M46+B47</f>
+        <f t="shared" ref="M47:M50" si="83">M46+B47</f>
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N49" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N50" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O49" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O50" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P49" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P50" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q49" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q50" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R49" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R50" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -4502,6 +4502,63 @@
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>45522</v>
+      </c>
+      <c r="B50">
+        <v>145434</v>
+      </c>
+      <c r="C50">
+        <v>6578</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>16519</v>
+      </c>
+      <c r="F50">
+        <v>9</v>
+      </c>
+      <c r="G50">
+        <v>30</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>31</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1">
+        <f t="shared" si="83"/>
+        <v>1302273</v>
+      </c>
+      <c r="N50" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="85"/>
+        <v>145465</v>
+      </c>
+      <c r="P50" s="1">
+        <f t="shared" si="86"/>
+        <v>1302633</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" si="87"/>
+        <v>6578</v>
+      </c>
+      <c r="R50" s="1">
+        <f t="shared" si="88"/>
+        <v>72303</v>
       </c>
       <c r="S50" s="1">
         <v>51083</v>

</xml_diff>

<commit_message>
8/21/24 updates - text needs update
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7B59CA-6DEB-714B-9288-8CF7F5B9CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6277BD-6293-7643-A693-28086FBA50A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1340" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="12540" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S51" sqref="S51"/>
+      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4273,27 +4273,27 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47:M51" si="83">M46+B47</f>
+        <f t="shared" ref="M47:M52" si="83">M46+B47</f>
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N51" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N52" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O51" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O52" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P51" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P52" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q51" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q52" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R51" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R52" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -4678,6 +4678,63 @@
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>45524</v>
+      </c>
+      <c r="B52">
+        <v>80112</v>
+      </c>
+      <c r="C52">
+        <v>2870</v>
+      </c>
+      <c r="D52">
+        <v>42</v>
+      </c>
+      <c r="E52">
+        <v>9730</v>
+      </c>
+      <c r="F52">
+        <v>32</v>
+      </c>
+      <c r="G52">
+        <v>37</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="1">
+        <f t="shared" si="83"/>
+        <v>1495420</v>
+      </c>
+      <c r="N52" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O52" s="2">
+        <f t="shared" si="85"/>
+        <v>80120</v>
+      </c>
+      <c r="P52" s="1">
+        <f t="shared" si="86"/>
+        <v>1495807</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" si="87"/>
+        <v>2870</v>
+      </c>
+      <c r="R52" s="1">
+        <f t="shared" si="88"/>
+        <v>80114</v>
       </c>
       <c r="S52" s="1">
         <v>36599</v>

</xml_diff>

<commit_message>
update Babine data 8/27
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E34DF6-A066-F243-8127-DEDFEFEC1B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2372C8FD-69BC-C346-9109-0418345EFE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15700" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="8220" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
+      <selection pane="bottomRight" activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4273,27 +4273,27 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47:M57" si="83">M46+B47</f>
+        <f t="shared" ref="M47:M58" si="83">M46+B47</f>
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N57" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N58" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O57" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O58" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P57" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P58" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q57" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q58" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R57" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R58" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -5206,6 +5206,63 @@
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>45530</v>
+      </c>
+      <c r="B58">
+        <v>41981</v>
+      </c>
+      <c r="C58">
+        <v>3441</v>
+      </c>
+      <c r="D58">
+        <v>94</v>
+      </c>
+      <c r="E58">
+        <v>5821</v>
+      </c>
+      <c r="F58">
+        <v>17</v>
+      </c>
+      <c r="G58">
+        <v>48</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>637</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1">
+        <f t="shared" si="83"/>
+        <v>1812418</v>
+      </c>
+      <c r="N58" s="1">
+        <f t="shared" si="84"/>
+        <v>637</v>
+      </c>
+      <c r="O58" s="2">
+        <f t="shared" si="85"/>
+        <v>42618</v>
+      </c>
+      <c r="P58" s="1">
+        <f t="shared" si="86"/>
+        <v>1817341</v>
+      </c>
+      <c r="Q58" s="1">
+        <f t="shared" si="87"/>
+        <v>3441</v>
+      </c>
+      <c r="R58" s="1">
+        <f t="shared" si="88"/>
+        <v>101163</v>
       </c>
       <c r="S58" s="1">
         <v>56160</v>

</xml_diff>

<commit_message>
update babine data to 8/28
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2372C8FD-69BC-C346-9109-0418345EFE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8704DC6F-ACCB-0D49-B6A2-346EA8142747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="6520" yWindow="500" windowWidth="22280" windowHeight="15440" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R62" sqref="R62"/>
+      <selection pane="bottomRight" activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4273,27 +4273,27 @@
         <v>0</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" ref="M47:M58" si="83">M46+B47</f>
+        <f t="shared" ref="M47:M59" si="83">M46+B47</f>
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N58" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N59" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O58" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O59" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P58" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P59" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q58" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q59" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R58" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R59" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -5294,6 +5294,63 @@
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>45531</v>
+      </c>
+      <c r="B59">
+        <v>19710</v>
+      </c>
+      <c r="C59">
+        <v>1661</v>
+      </c>
+      <c r="D59">
+        <v>50</v>
+      </c>
+      <c r="E59">
+        <v>2990</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+      <c r="G59">
+        <v>16</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59" s="1">
+        <f t="shared" si="83"/>
+        <v>1832128</v>
+      </c>
+      <c r="N59" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O59" s="2">
+        <f t="shared" si="85"/>
+        <v>19712</v>
+      </c>
+      <c r="P59" s="1">
+        <f t="shared" si="86"/>
+        <v>1837053</v>
+      </c>
+      <c r="Q59" s="1">
+        <f t="shared" si="87"/>
+        <v>1661</v>
+      </c>
+      <c r="R59" s="1">
+        <f t="shared" si="88"/>
+        <v>102824</v>
       </c>
       <c r="S59" s="1">
         <v>43271</v>

</xml_diff>

<commit_message>
8/30 with Babine updates
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F48C034-81EB-1D45-A7E6-4427259635BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEB1AAD-992A-EB48-BB90-45AE00EB38CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P60" sqref="P60"/>
+      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4277,23 +4277,23 @@
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N60" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N61" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O60" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O61" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P60" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P61" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q60" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q61" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R60" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R61" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -5470,6 +5470,63 @@
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>45533</v>
+      </c>
+      <c r="B61">
+        <v>21451</v>
+      </c>
+      <c r="C61">
+        <v>2597</v>
+      </c>
+      <c r="D61">
+        <v>107</v>
+      </c>
+      <c r="E61">
+        <v>4500</v>
+      </c>
+      <c r="F61">
+        <v>24</v>
+      </c>
+      <c r="G61">
+        <v>23</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" s="1">
+        <f>M60+B61</f>
+        <v>1880626</v>
+      </c>
+      <c r="N61" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O61" s="2">
+        <f t="shared" si="85"/>
+        <v>21451</v>
+      </c>
+      <c r="P61" s="1">
+        <f t="shared" si="86"/>
+        <v>1886007</v>
+      </c>
+      <c r="Q61" s="1">
+        <f t="shared" si="87"/>
+        <v>2597</v>
+      </c>
+      <c r="R61" s="1">
+        <f t="shared" si="88"/>
+        <v>108266</v>
       </c>
       <c r="S61" s="1">
         <v>48129</v>

</xml_diff>

<commit_message>
add table with Babine fence sockeye/TRTC estimate
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F109A-820A-4647-8504-52902EC53ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7D2314-0814-FA47-8ADF-F0C5602C26E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q64" sqref="Q64"/>
+      <selection pane="bottomRight" activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4277,23 +4277,23 @@
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N65" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N66" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O65" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O66" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P65" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P66" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q65" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q66" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R65" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R66" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -5769,7 +5769,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" ref="M64:M65" si="90">M63+B64</f>
+        <f t="shared" ref="M64:M66" si="90">M63+B64</f>
         <v>1922769</v>
       </c>
       <c r="N64" s="1">
@@ -5910,6 +5910,63 @@
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>45538</v>
+      </c>
+      <c r="B66">
+        <v>7512</v>
+      </c>
+      <c r="C66">
+        <v>1319</v>
+      </c>
+      <c r="D66">
+        <v>131</v>
+      </c>
+      <c r="E66">
+        <v>2943</v>
+      </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>730</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" s="1">
+        <f t="shared" si="90"/>
+        <v>1937292</v>
+      </c>
+      <c r="N66" s="1">
+        <f t="shared" si="84"/>
+        <v>730</v>
+      </c>
+      <c r="O66" s="2">
+        <f t="shared" si="85"/>
+        <v>8242</v>
+      </c>
+      <c r="P66" s="1">
+        <f t="shared" si="86"/>
+        <v>1945411</v>
+      </c>
+      <c r="Q66" s="1">
+        <f t="shared" si="87"/>
+        <v>1319</v>
+      </c>
+      <c r="R66" s="1">
+        <f t="shared" si="88"/>
+        <v>117477</v>
       </c>
       <c r="S66" s="1">
         <v>26054</v>

</xml_diff>

<commit_message>
daily updates Sept. 11
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFAC589-3514-3446-94E9-D0FFCA58986E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60E3AC8-69DB-024C-8CFB-7C0C834315F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="10300" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q75" sqref="Q75"/>
+      <selection pane="bottomRight" activeCell="Q70" sqref="Q70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4277,23 +4277,23 @@
         <v>963894</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" ref="N47:N71" si="84">J47+L47</f>
+        <f t="shared" ref="N47:N73" si="84">J47+L47</f>
         <v>0</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" ref="O47:O71" si="85">B47+I47+N47</f>
+        <f t="shared" ref="O47:O73" si="85">B47+I47+N47</f>
         <v>45949</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" ref="P47:P71" si="86">P46+O47</f>
+        <f t="shared" ref="P47:P73" si="86">P46+O47</f>
         <v>964161</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q71" si="87">C47+K47</f>
+        <f t="shared" ref="Q47:Q73" si="87">C47+K47</f>
         <v>3035</v>
       </c>
       <c r="R47" s="1">
-        <f t="shared" ref="R47:R71" si="88">Q47+R46</f>
+        <f t="shared" ref="R47:R73" si="88">Q47+R46</f>
         <v>57072</v>
       </c>
       <c r="S47" s="1">
@@ -5769,7 +5769,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="1">
-        <f t="shared" ref="M64:M71" si="90">M63+B64</f>
+        <f t="shared" ref="M64:M73" si="90">M63+B64</f>
         <v>1922769</v>
       </c>
       <c r="N64" s="1">
@@ -6439,6 +6439,63 @@
       <c r="A72" s="3">
         <v>45544</v>
       </c>
+      <c r="B72">
+        <v>5248</v>
+      </c>
+      <c r="C72">
+        <v>450</v>
+      </c>
+      <c r="D72">
+        <v>260</v>
+      </c>
+      <c r="E72">
+        <v>6580</v>
+      </c>
+      <c r="F72">
+        <v>78</v>
+      </c>
+      <c r="G72">
+        <v>39</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" s="1">
+        <f t="shared" si="90"/>
+        <v>1975053</v>
+      </c>
+      <c r="N72" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O72" s="2">
+        <f t="shared" si="85"/>
+        <v>5248</v>
+      </c>
+      <c r="P72" s="1">
+        <f t="shared" si="86"/>
+        <v>1984183</v>
+      </c>
+      <c r="Q72" s="1">
+        <f t="shared" si="87"/>
+        <v>450</v>
+      </c>
+      <c r="R72" s="1">
+        <f t="shared" si="88"/>
+        <v>124247</v>
+      </c>
       <c r="S72" s="1">
         <v>13635</v>
       </c>
@@ -6469,6 +6526,63 @@
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>45545</v>
+      </c>
+      <c r="B73">
+        <v>3708</v>
+      </c>
+      <c r="C73">
+        <v>448</v>
+      </c>
+      <c r="D73">
+        <v>367</v>
+      </c>
+      <c r="E73">
+        <v>6326</v>
+      </c>
+      <c r="F73">
+        <v>26</v>
+      </c>
+      <c r="G73">
+        <v>29</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73" s="1">
+        <f t="shared" si="90"/>
+        <v>1978761</v>
+      </c>
+      <c r="N73" s="1">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="O73" s="2">
+        <f t="shared" si="85"/>
+        <v>3708</v>
+      </c>
+      <c r="P73" s="1">
+        <f t="shared" si="86"/>
+        <v>1987891</v>
+      </c>
+      <c r="Q73" s="1">
+        <f t="shared" si="87"/>
+        <v>448</v>
+      </c>
+      <c r="R73" s="1">
+        <f t="shared" si="88"/>
+        <v>124695</v>
       </c>
       <c r="S73" s="1">
         <v>9796</v>

</xml_diff>

<commit_message>
October 1 update for Babine fence counts (Tyee data up to Sept 23)
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2613B17-EFAA-204B-A1F4-BC30FB215D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E43653-E0F6-474C-AEB5-DC5A4C88D4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="8880" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R88" sqref="R88"/>
+      <selection pane="bottomRight" activeCell="U91" sqref="U91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7671,6 +7671,63 @@
       <c r="A86" s="3">
         <v>45558</v>
       </c>
+      <c r="B86">
+        <v>2139</v>
+      </c>
+      <c r="C86">
+        <v>385</v>
+      </c>
+      <c r="D86">
+        <v>217</v>
+      </c>
+      <c r="E86">
+        <v>4053</v>
+      </c>
+      <c r="F86">
+        <v>85</v>
+      </c>
+      <c r="G86">
+        <v>52</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" s="1">
+        <f t="shared" ref="M86:M93" si="94">M85+B86</f>
+        <v>2004693</v>
+      </c>
+      <c r="N86" s="1">
+        <f t="shared" ref="N86:N93" si="95">J86+L86</f>
+        <v>0</v>
+      </c>
+      <c r="O86" s="2">
+        <f t="shared" ref="O86:O93" si="96">B86+I86+N86</f>
+        <v>2139</v>
+      </c>
+      <c r="P86" s="1">
+        <f t="shared" ref="P86:P93" si="97">P85+O86</f>
+        <v>2013824</v>
+      </c>
+      <c r="Q86" s="1">
+        <f t="shared" ref="Q86:Q93" si="98">C86+K86</f>
+        <v>385</v>
+      </c>
+      <c r="R86" s="1">
+        <f t="shared" ref="R86:R93" si="99">Q86+R85</f>
+        <v>127973</v>
+      </c>
       <c r="S86" s="1">
         <v>3729</v>
       </c>
@@ -7702,6 +7759,63 @@
       <c r="A87" s="3">
         <v>45559</v>
       </c>
+      <c r="B87">
+        <v>895</v>
+      </c>
+      <c r="C87">
+        <v>230</v>
+      </c>
+      <c r="D87">
+        <v>203</v>
+      </c>
+      <c r="E87">
+        <v>2360</v>
+      </c>
+      <c r="F87">
+        <v>115</v>
+      </c>
+      <c r="G87">
+        <v>57</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87" s="1">
+        <f t="shared" si="94"/>
+        <v>2005588</v>
+      </c>
+      <c r="N87" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O87" s="2">
+        <f t="shared" si="96"/>
+        <v>895</v>
+      </c>
+      <c r="P87" s="1">
+        <f t="shared" si="97"/>
+        <v>2014719</v>
+      </c>
+      <c r="Q87" s="1">
+        <f t="shared" si="98"/>
+        <v>230</v>
+      </c>
+      <c r="R87" s="1">
+        <f t="shared" si="99"/>
+        <v>128203</v>
+      </c>
       <c r="S87" s="1">
         <v>2655</v>
       </c>
@@ -7733,6 +7847,63 @@
       <c r="A88" s="3">
         <v>45560</v>
       </c>
+      <c r="B88">
+        <v>515</v>
+      </c>
+      <c r="C88">
+        <v>216</v>
+      </c>
+      <c r="D88">
+        <v>103</v>
+      </c>
+      <c r="E88">
+        <v>1713</v>
+      </c>
+      <c r="F88">
+        <v>78</v>
+      </c>
+      <c r="G88">
+        <v>123</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88" s="1">
+        <f t="shared" si="94"/>
+        <v>2006103</v>
+      </c>
+      <c r="N88" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O88" s="2">
+        <f t="shared" si="96"/>
+        <v>515</v>
+      </c>
+      <c r="P88" s="1">
+        <f t="shared" si="97"/>
+        <v>2015234</v>
+      </c>
+      <c r="Q88" s="1">
+        <f t="shared" si="98"/>
+        <v>216</v>
+      </c>
+      <c r="R88" s="1">
+        <f t="shared" si="99"/>
+        <v>128419</v>
+      </c>
       <c r="S88" s="1">
         <v>1998</v>
       </c>
@@ -7764,6 +7935,63 @@
       <c r="A89" s="3">
         <v>45561</v>
       </c>
+      <c r="B89">
+        <v>504</v>
+      </c>
+      <c r="C89">
+        <v>146</v>
+      </c>
+      <c r="D89">
+        <v>90</v>
+      </c>
+      <c r="E89">
+        <v>1122</v>
+      </c>
+      <c r="F89">
+        <v>51</v>
+      </c>
+      <c r="G89">
+        <v>82</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89" s="1">
+        <f t="shared" si="94"/>
+        <v>2006607</v>
+      </c>
+      <c r="N89" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O89" s="2">
+        <f t="shared" si="96"/>
+        <v>504</v>
+      </c>
+      <c r="P89" s="1">
+        <f t="shared" si="97"/>
+        <v>2015738</v>
+      </c>
+      <c r="Q89" s="1">
+        <f t="shared" si="98"/>
+        <v>146</v>
+      </c>
+      <c r="R89" s="1">
+        <f t="shared" si="99"/>
+        <v>128565</v>
+      </c>
       <c r="S89" s="1">
         <v>1292</v>
       </c>
@@ -7795,6 +8023,63 @@
       <c r="A90" s="3">
         <v>45562</v>
       </c>
+      <c r="B90">
+        <v>215</v>
+      </c>
+      <c r="C90">
+        <v>69</v>
+      </c>
+      <c r="D90">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>590</v>
+      </c>
+      <c r="F90">
+        <v>28</v>
+      </c>
+      <c r="G90">
+        <v>40</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" s="1">
+        <f t="shared" si="94"/>
+        <v>2006822</v>
+      </c>
+      <c r="N90" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O90" s="2">
+        <f t="shared" si="96"/>
+        <v>215</v>
+      </c>
+      <c r="P90" s="1">
+        <f t="shared" si="97"/>
+        <v>2015953</v>
+      </c>
+      <c r="Q90" s="1">
+        <f t="shared" si="98"/>
+        <v>69</v>
+      </c>
+      <c r="R90" s="1">
+        <f t="shared" si="99"/>
+        <v>128634</v>
+      </c>
       <c r="S90" s="1">
         <v>829</v>
       </c>
@@ -7826,6 +8111,63 @@
       <c r="A91" s="3">
         <v>45563</v>
       </c>
+      <c r="B91">
+        <v>77</v>
+      </c>
+      <c r="C91">
+        <v>20</v>
+      </c>
+      <c r="D91">
+        <v>7</v>
+      </c>
+      <c r="E91">
+        <v>164</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91" s="1">
+        <f t="shared" si="94"/>
+        <v>2006899</v>
+      </c>
+      <c r="N91" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O91" s="2">
+        <f t="shared" si="96"/>
+        <v>77</v>
+      </c>
+      <c r="P91" s="1">
+        <f t="shared" si="97"/>
+        <v>2016030</v>
+      </c>
+      <c r="Q91" s="1">
+        <f t="shared" si="98"/>
+        <v>20</v>
+      </c>
+      <c r="R91" s="1">
+        <f t="shared" si="99"/>
+        <v>128654</v>
+      </c>
       <c r="S91" s="1">
         <v>1168</v>
       </c>
@@ -7857,6 +8199,63 @@
       <c r="A92" s="3">
         <v>45564</v>
       </c>
+      <c r="B92">
+        <v>60</v>
+      </c>
+      <c r="C92">
+        <v>15</v>
+      </c>
+      <c r="D92">
+        <v>16</v>
+      </c>
+      <c r="E92">
+        <v>108</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>15</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" s="1">
+        <f t="shared" si="94"/>
+        <v>2006959</v>
+      </c>
+      <c r="N92" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O92" s="2">
+        <f t="shared" si="96"/>
+        <v>60</v>
+      </c>
+      <c r="P92" s="1">
+        <f t="shared" si="97"/>
+        <v>2016090</v>
+      </c>
+      <c r="Q92" s="1">
+        <f t="shared" si="98"/>
+        <v>15</v>
+      </c>
+      <c r="R92" s="1">
+        <f t="shared" si="99"/>
+        <v>128669</v>
+      </c>
       <c r="S92" s="1">
         <v>935</v>
       </c>
@@ -7888,6 +8287,63 @@
       <c r="A93" s="3">
         <v>45565</v>
       </c>
+      <c r="B93">
+        <v>79</v>
+      </c>
+      <c r="C93">
+        <v>13</v>
+      </c>
+      <c r="D93">
+        <v>12</v>
+      </c>
+      <c r="E93">
+        <v>63</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>11</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93" s="1">
+        <f t="shared" si="94"/>
+        <v>2007038</v>
+      </c>
+      <c r="N93" s="1">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="O93" s="2">
+        <f t="shared" si="96"/>
+        <v>79</v>
+      </c>
+      <c r="P93" s="1">
+        <f t="shared" si="97"/>
+        <v>2016169</v>
+      </c>
+      <c r="Q93" s="1">
+        <f t="shared" si="98"/>
+        <v>13</v>
+      </c>
+      <c r="R93" s="1">
+        <f t="shared" si="99"/>
+        <v>128682</v>
+      </c>
       <c r="S93" s="1">
         <v>896</v>
       </c>
@@ -8088,11 +8544,11 @@
         <v>45572</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" ref="U100:V108" si="94">U99+S100</f>
+        <f t="shared" ref="U100:V108" si="100">U99+S100</f>
         <v>2052845</v>
       </c>
       <c r="V100" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W100" s="1">
@@ -8113,11 +8569,11 @@
         <v>45573</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V101" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W101" s="1">
@@ -8132,11 +8588,11 @@
         <v>45574</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V102" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W102" s="1">
@@ -8151,11 +8607,11 @@
         <v>45575</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V103" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W103" s="1">
@@ -8170,11 +8626,11 @@
         <v>45576</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V104" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W104" s="1">
@@ -8189,11 +8645,11 @@
         <v>45577</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V105" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W105" s="1">
@@ -8208,11 +8664,11 @@
         <v>45578</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V106" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W106" s="1">
@@ -8227,11 +8683,11 @@
         <v>45579</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V107" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W107" s="1">
@@ -8246,11 +8702,11 @@
         <v>45580</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>2052845</v>
       </c>
       <c r="V108" s="1">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W108" s="1">

</xml_diff>

<commit_message>
update Babine fence counts 10/7
</commit_message>
<xml_diff>
--- a/data/babine data 2024.xlsx
+++ b/data/babine data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E43653-E0F6-474C-AEB5-DC5A4C88D4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D6B48C-1F2B-D645-8805-27D7074B5D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
+    <workbookView xWindow="11300" yWindow="500" windowWidth="22280" windowHeight="13260" xr2:uid="{52AE178B-9CC6-4B68-8B92-85EF0B36AB16}"/>
   </bookViews>
   <sheets>
     <sheet name="Babine" sheetId="1" r:id="rId1"/>
@@ -500,10 +500,10 @@
   <dimension ref="A1:Z108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U91" sqref="U91"/>
+      <selection pane="bottomRight" activeCell="Q100" sqref="Q100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8375,12 +8375,72 @@
       <c r="A94" s="3">
         <v>45566</v>
       </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+      <c r="C94">
+        <v>15</v>
+      </c>
+      <c r="D94">
+        <v>17</v>
+      </c>
+      <c r="E94">
+        <v>59</v>
+      </c>
+      <c r="F94">
+        <v>4</v>
+      </c>
+      <c r="G94">
+        <v>5</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94" s="1">
+        <f t="shared" ref="M94:M97" si="100">M93+B94</f>
+        <v>2007098</v>
+      </c>
+      <c r="N94" s="1">
+        <f t="shared" ref="N94:N97" si="101">J94+L94</f>
+        <v>0</v>
+      </c>
+      <c r="O94" s="2">
+        <f t="shared" ref="O94:O97" si="102">B94+I94+N94</f>
+        <v>60</v>
+      </c>
+      <c r="P94" s="1">
+        <f t="shared" ref="P94:P97" si="103">P93+O94</f>
+        <v>2016229</v>
+      </c>
+      <c r="Q94" s="1">
+        <f t="shared" ref="Q94:Q97" si="104">C94+K94</f>
+        <v>15</v>
+      </c>
+      <c r="R94" s="1">
+        <f t="shared" ref="R94:R97" si="105">Q94+R93</f>
+        <v>128697</v>
+      </c>
+      <c r="S94" s="1">
+        <v>897</v>
+      </c>
       <c r="T94" s="1">
         <v>707.66666666666663</v>
       </c>
       <c r="U94" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2053742</v>
       </c>
       <c r="V94" s="1">
         <f t="shared" si="93"/>
@@ -8403,12 +8463,72 @@
       <c r="A95" s="3">
         <v>45567</v>
       </c>
+      <c r="B95">
+        <v>62</v>
+      </c>
+      <c r="C95">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <v>8</v>
+      </c>
+      <c r="E95">
+        <v>23</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95" s="1">
+        <f t="shared" si="100"/>
+        <v>2007160</v>
+      </c>
+      <c r="N95" s="1">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="O95" s="2">
+        <f t="shared" si="102"/>
+        <v>62</v>
+      </c>
+      <c r="P95" s="1">
+        <f t="shared" si="103"/>
+        <v>2016291</v>
+      </c>
+      <c r="Q95" s="1">
+        <f t="shared" si="104"/>
+        <v>10</v>
+      </c>
+      <c r="R95" s="1">
+        <f t="shared" si="105"/>
+        <v>128707</v>
+      </c>
+      <c r="S95" s="1">
+        <v>898</v>
+      </c>
       <c r="T95" s="1">
         <v>440</v>
       </c>
       <c r="U95" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2054640</v>
       </c>
       <c r="V95" s="1">
         <f t="shared" si="93"/>
@@ -8431,12 +8551,72 @@
       <c r="A96" s="3">
         <v>45568</v>
       </c>
+      <c r="B96">
+        <v>60</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96">
+        <v>15</v>
+      </c>
+      <c r="E96">
+        <v>9</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96" s="1">
+        <f t="shared" si="100"/>
+        <v>2007220</v>
+      </c>
+      <c r="N96" s="1">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="O96" s="2">
+        <f t="shared" si="102"/>
+        <v>60</v>
+      </c>
+      <c r="P96" s="1">
+        <f t="shared" si="103"/>
+        <v>2016351</v>
+      </c>
+      <c r="Q96" s="1">
+        <f t="shared" si="104"/>
+        <v>5</v>
+      </c>
+      <c r="R96" s="1">
+        <f t="shared" si="105"/>
+        <v>128712</v>
+      </c>
+      <c r="S96" s="1">
+        <v>899</v>
+      </c>
       <c r="T96" s="1">
         <v>720.66666666666663</v>
       </c>
       <c r="U96" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2055539</v>
       </c>
       <c r="V96" s="1">
         <f t="shared" si="93"/>
@@ -8459,12 +8639,72 @@
       <c r="A97" s="3">
         <v>45569</v>
       </c>
+      <c r="B97">
+        <v>48</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>15</v>
+      </c>
+      <c r="E97">
+        <v>11</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97" s="1">
+        <f t="shared" si="100"/>
+        <v>2007268</v>
+      </c>
+      <c r="N97" s="1">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="O97" s="2">
+        <f t="shared" si="102"/>
+        <v>48</v>
+      </c>
+      <c r="P97" s="1">
+        <f t="shared" si="103"/>
+        <v>2016399</v>
+      </c>
+      <c r="Q97" s="1">
+        <f t="shared" si="104"/>
+        <v>2</v>
+      </c>
+      <c r="R97" s="1">
+        <f t="shared" si="105"/>
+        <v>128714</v>
+      </c>
+      <c r="S97" s="1">
+        <v>900</v>
+      </c>
       <c r="T97" s="1">
         <v>238</v>
       </c>
       <c r="U97" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2056439</v>
       </c>
       <c r="V97" s="1">
         <f t="shared" si="93"/>
@@ -8492,7 +8732,7 @@
       </c>
       <c r="U98" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2056439</v>
       </c>
       <c r="V98" s="1">
         <f t="shared" si="93"/>
@@ -8520,7 +8760,7 @@
       </c>
       <c r="U99" s="1">
         <f t="shared" si="93"/>
-        <v>2052845</v>
+        <v>2056439</v>
       </c>
       <c r="V99" s="1">
         <f t="shared" si="93"/>
@@ -8544,11 +8784,11 @@
         <v>45572</v>
       </c>
       <c r="U100" s="1">
-        <f t="shared" ref="U100:V108" si="100">U99+S100</f>
-        <v>2052845</v>
+        <f t="shared" ref="U100:V108" si="106">U99+S100</f>
+        <v>2056439</v>
       </c>
       <c r="V100" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W100" s="1">
@@ -8569,11 +8809,11 @@
         <v>45573</v>
       </c>
       <c r="U101" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V101" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W101" s="1">
@@ -8588,11 +8828,11 @@
         <v>45574</v>
       </c>
       <c r="U102" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V102" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W102" s="1">
@@ -8607,11 +8847,11 @@
         <v>45575</v>
       </c>
       <c r="U103" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V103" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W103" s="1">
@@ -8626,11 +8866,11 @@
         <v>45576</v>
       </c>
       <c r="U104" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V104" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W104" s="1">
@@ -8645,11 +8885,11 @@
         <v>45577</v>
       </c>
       <c r="U105" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V105" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W105" s="1">
@@ -8664,11 +8904,11 @@
         <v>45578</v>
       </c>
       <c r="U106" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V106" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W106" s="1">
@@ -8683,11 +8923,11 @@
         <v>45579</v>
       </c>
       <c r="U107" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V107" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W107" s="1">
@@ -8702,11 +8942,11 @@
         <v>45580</v>
       </c>
       <c r="U108" s="1">
-        <f t="shared" si="100"/>
-        <v>2052845</v>
+        <f t="shared" si="106"/>
+        <v>2056439</v>
       </c>
       <c r="V108" s="1">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>1128680.6570346321</v>
       </c>
       <c r="W108" s="1">

</xml_diff>